<commit_message>
Added priority columns for geologie and bodem
</commit_message>
<xml_diff>
--- a/data/bodem_template.xlsx
+++ b/data/bodem_template.xlsx
@@ -40748,9 +40748,9 @@
     <col min="28" max="28" width="112.7109375" hidden="1" customWidth="1"/>
     <col min="29" max="29" width="108.7109375" hidden="1" customWidth="1"/>
     <col min="30" max="30" width="64.7109375" style="2" hidden="1" customWidth="1"/>
-    <col min="31" max="32" width="42.7109375" hidden="1" customWidth="1"/>
-    <col min="33" max="34" width="70.7109375" hidden="1" customWidth="1"/>
-    <col min="35" max="35" width="98.7109375" hidden="1" customWidth="1"/>
+    <col min="31" max="32" width="42.7109375" customWidth="1"/>
+    <col min="33" max="34" width="70.7109375" customWidth="1"/>
+    <col min="35" max="35" width="98.7109375" customWidth="1"/>
     <col min="36" max="36" width="130.7109375" hidden="1" customWidth="1"/>
     <col min="37" max="37" width="132.7109375" hidden="1" customWidth="1"/>
     <col min="38" max="38" width="144.7109375" hidden="1" customWidth="1"/>
@@ -40759,9 +40759,9 @@
     <col min="41" max="41" width="116.7109375" hidden="1" customWidth="1"/>
     <col min="42" max="42" width="98.7109375" hidden="1" customWidth="1"/>
     <col min="43" max="43" width="94.7109375" hidden="1" customWidth="1"/>
-    <col min="44" max="44" width="64.7109375" hidden="1" customWidth="1"/>
-    <col min="45" max="46" width="82.7109375" hidden="1" customWidth="1"/>
-    <col min="47" max="47" width="110.7109375" hidden="1" customWidth="1"/>
+    <col min="44" max="44" width="64.7109375" customWidth="1"/>
+    <col min="45" max="46" width="82.7109375" customWidth="1"/>
+    <col min="47" max="47" width="110.7109375" customWidth="1"/>
     <col min="48" max="48" width="142.7109375" hidden="1" customWidth="1"/>
     <col min="49" max="49" width="144.7109375" hidden="1" customWidth="1"/>
     <col min="50" max="50" width="156.7109375" hidden="1" customWidth="1"/>
@@ -40770,24 +40770,25 @@
     <col min="53" max="53" width="128.7109375" hidden="1" customWidth="1"/>
     <col min="54" max="54" width="110.7109375" hidden="1" customWidth="1"/>
     <col min="55" max="55" width="106.7109375" hidden="1" customWidth="1"/>
-    <col min="56" max="56" width="62.7109375" style="2" hidden="1" customWidth="1"/>
+    <col min="56" max="56" width="62.7109375" style="2" customWidth="1"/>
     <col min="57" max="57" width="38.7109375" hidden="1" customWidth="1"/>
     <col min="58" max="58" width="42.7109375" hidden="1" customWidth="1"/>
     <col min="59" max="60" width="44.7109375" hidden="1" customWidth="1"/>
-    <col min="61" max="62" width="40.7109375" hidden="1" customWidth="1"/>
-    <col min="63" max="63" width="44.7109375" hidden="1" customWidth="1"/>
-    <col min="64" max="64" width="36.7109375" hidden="1" customWidth="1"/>
+    <col min="61" max="61" width="40.7109375" customWidth="1"/>
+    <col min="62" max="62" width="40.7109375" hidden="1" customWidth="1"/>
+    <col min="63" max="63" width="44.7109375" customWidth="1"/>
+    <col min="64" max="64" width="36.7109375" customWidth="1"/>
     <col min="65" max="65" width="22.7109375" style="2" hidden="1" customWidth="1"/>
     <col min="66" max="66" width="34.7109375" hidden="1" customWidth="1"/>
     <col min="67" max="67" width="24.7109375" hidden="1" customWidth="1"/>
     <col min="68" max="68" width="40.7109375" hidden="1" customWidth="1"/>
-    <col min="69" max="69" width="12.7109375" hidden="1" customWidth="1"/>
+    <col min="69" max="69" width="12.7109375" customWidth="1"/>
     <col min="70" max="70" width="56.7109375" hidden="1" customWidth="1"/>
     <col min="71" max="71" width="64.7109375" hidden="1" customWidth="1"/>
     <col min="72" max="72" width="76.7109375" hidden="1" customWidth="1"/>
     <col min="73" max="73" width="58.7109375" hidden="1" customWidth="1"/>
     <col min="74" max="74" width="54.7109375" hidden="1" customWidth="1"/>
-    <col min="75" max="75" width="74.7109375" hidden="1" customWidth="1"/>
+    <col min="75" max="75" width="74.7109375" customWidth="1"/>
     <col min="76" max="76" width="106.7109375" hidden="1" customWidth="1"/>
     <col min="77" max="77" width="108.7109375" hidden="1" customWidth="1"/>
     <col min="78" max="78" width="120.7109375" hidden="1" customWidth="1"/>
@@ -40797,12 +40798,12 @@
     <col min="82" max="82" width="74.7109375" hidden="1" customWidth="1"/>
     <col min="83" max="83" width="70.7109375" hidden="1" customWidth="1"/>
     <col min="84" max="85" width="20.7109375" hidden="1" customWidth="1"/>
-    <col min="86" max="86" width="38.7109375" hidden="1" customWidth="1"/>
-    <col min="87" max="87" width="46.7109375" hidden="1" customWidth="1"/>
+    <col min="86" max="86" width="38.7109375" customWidth="1"/>
+    <col min="87" max="87" width="46.7109375" customWidth="1"/>
     <col min="88" max="88" width="58.7109375" hidden="1" customWidth="1"/>
     <col min="89" max="89" width="40.7109375" hidden="1" customWidth="1"/>
     <col min="90" max="90" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="91" max="91" width="56.7109375" hidden="1" customWidth="1"/>
+    <col min="91" max="91" width="56.7109375" customWidth="1"/>
     <col min="92" max="92" width="88.7109375" hidden="1" customWidth="1"/>
     <col min="93" max="93" width="90.7109375" hidden="1" customWidth="1"/>
     <col min="94" max="94" width="102.7109375" hidden="1" customWidth="1"/>
@@ -40811,23 +40812,23 @@
     <col min="97" max="97" width="74.7109375" hidden="1" customWidth="1"/>
     <col min="98" max="98" width="56.7109375" hidden="1" customWidth="1"/>
     <col min="99" max="99" width="52.7109375" hidden="1" customWidth="1"/>
-    <col min="100" max="100" width="30.7109375" hidden="1" customWidth="1"/>
-    <col min="101" max="101" width="42.7109375" hidden="1" customWidth="1"/>
-    <col min="102" max="102" width="50.7109375" hidden="1" customWidth="1"/>
+    <col min="100" max="100" width="30.7109375" customWidth="1"/>
+    <col min="101" max="101" width="42.7109375" customWidth="1"/>
+    <col min="102" max="102" width="50.7109375" customWidth="1"/>
     <col min="103" max="103" width="62.7109375" hidden="1" customWidth="1"/>
     <col min="104" max="104" width="44.7109375" hidden="1" customWidth="1"/>
     <col min="105" max="105" width="40.7109375" hidden="1" customWidth="1"/>
-    <col min="106" max="106" width="30.7109375" style="2" hidden="1" customWidth="1"/>
-    <col min="107" max="107" width="16.7109375" hidden="1" customWidth="1"/>
-    <col min="108" max="108" width="26.7109375" hidden="1" customWidth="1"/>
-    <col min="109" max="109" width="44.7109375" style="2" hidden="1" customWidth="1"/>
-    <col min="110" max="110" width="42.7109375" hidden="1" customWidth="1"/>
-    <col min="111" max="111" width="48.7109375" hidden="1" customWidth="1"/>
-    <col min="112" max="112" width="40.7109375" hidden="1" customWidth="1"/>
-    <col min="113" max="113" width="30.7109375" hidden="1" customWidth="1"/>
-    <col min="114" max="114" width="40.7109375" hidden="1" customWidth="1"/>
-    <col min="115" max="115" width="34.7109375" hidden="1" customWidth="1"/>
-    <col min="116" max="116" width="36.7109375" hidden="1" customWidth="1"/>
+    <col min="106" max="106" width="30.7109375" style="2" customWidth="1"/>
+    <col min="107" max="107" width="16.7109375" customWidth="1"/>
+    <col min="108" max="108" width="26.7109375" customWidth="1"/>
+    <col min="109" max="109" width="44.7109375" style="2" customWidth="1"/>
+    <col min="110" max="110" width="42.7109375" customWidth="1"/>
+    <col min="111" max="111" width="48.7109375" customWidth="1"/>
+    <col min="112" max="112" width="40.7109375" customWidth="1"/>
+    <col min="113" max="113" width="30.7109375" customWidth="1"/>
+    <col min="114" max="114" width="40.7109375" customWidth="1"/>
+    <col min="115" max="115" width="34.7109375" customWidth="1"/>
+    <col min="116" max="116" width="36.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:116" hidden="1">
@@ -42482,20 +42483,20 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.7109375" customWidth="1"/>
-    <col min="2" max="2" width="44.7109375" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" style="2" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" style="2" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="56.7109375" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="26.7109375" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="38.7109375" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="46.7109375" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="44.7109375" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" customWidth="1"/>
+    <col min="4" max="4" width="32.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" customWidth="1"/>
+    <col min="7" max="7" width="56.7109375" customWidth="1"/>
+    <col min="8" max="8" width="26.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="38.7109375" customWidth="1"/>
+    <col min="11" max="11" width="46.7109375" customWidth="1"/>
     <col min="12" max="12" width="58.7109375" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="40.7109375" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="56.7109375" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="56.7109375" customWidth="1"/>
     <col min="16" max="16" width="88.7109375" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="90.7109375" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="102.7109375" hidden="1" customWidth="1"/>
@@ -42504,22 +42505,22 @@
     <col min="21" max="21" width="74.7109375" hidden="1" customWidth="1"/>
     <col min="22" max="22" width="56.7109375" hidden="1" customWidth="1"/>
     <col min="23" max="23" width="52.7109375" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="30.7109375" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="42.7109375" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="50.7109375" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="30.7109375" customWidth="1"/>
+    <col min="25" max="25" width="42.7109375" customWidth="1"/>
+    <col min="26" max="26" width="50.7109375" customWidth="1"/>
     <col min="27" max="27" width="62.7109375" hidden="1" customWidth="1"/>
     <col min="28" max="28" width="44.7109375" hidden="1" customWidth="1"/>
     <col min="29" max="29" width="40.7109375" hidden="1" customWidth="1"/>
-    <col min="30" max="30" width="30.7109375" style="2" hidden="1" customWidth="1"/>
-    <col min="31" max="31" width="16.7109375" hidden="1" customWidth="1"/>
-    <col min="32" max="32" width="26.7109375" hidden="1" customWidth="1"/>
-    <col min="33" max="33" width="44.7109375" style="2" hidden="1" customWidth="1"/>
-    <col min="34" max="34" width="42.7109375" hidden="1" customWidth="1"/>
-    <col min="35" max="35" width="48.7109375" hidden="1" customWidth="1"/>
-    <col min="36" max="36" width="40.7109375" hidden="1" customWidth="1"/>
-    <col min="37" max="37" width="30.7109375" hidden="1" customWidth="1"/>
-    <col min="38" max="38" width="40.7109375" hidden="1" customWidth="1"/>
-    <col min="39" max="39" width="34.7109375" hidden="1" customWidth="1"/>
+    <col min="30" max="30" width="30.7109375" style="2" customWidth="1"/>
+    <col min="31" max="31" width="16.7109375" customWidth="1"/>
+    <col min="32" max="32" width="26.7109375" customWidth="1"/>
+    <col min="33" max="33" width="44.7109375" style="2" customWidth="1"/>
+    <col min="34" max="34" width="42.7109375" customWidth="1"/>
+    <col min="35" max="35" width="48.7109375" customWidth="1"/>
+    <col min="36" max="36" width="40.7109375" customWidth="1"/>
+    <col min="37" max="37" width="30.7109375" customWidth="1"/>
+    <col min="38" max="38" width="40.7109375" customWidth="1"/>
+    <col min="39" max="39" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:39" hidden="1">
@@ -43041,54 +43042,54 @@
     <col min="6" max="6" width="98.7109375" customWidth="1"/>
     <col min="7" max="7" width="64.7109375" customWidth="1"/>
     <col min="8" max="8" width="76.7109375" customWidth="1"/>
-    <col min="9" max="9" width="44.7109375" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="40.7109375" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="58.7109375" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="90.7109375" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="92.7109375" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="104.7109375" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="56.7109375" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="64.7109375" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="44.7109375" customWidth="1"/>
+    <col min="10" max="10" width="36.7109375" customWidth="1"/>
+    <col min="11" max="11" width="40.7109375" customWidth="1"/>
+    <col min="12" max="12" width="58.7109375" customWidth="1"/>
+    <col min="13" max="13" width="90.7109375" customWidth="1"/>
+    <col min="14" max="14" width="92.7109375" customWidth="1"/>
+    <col min="15" max="15" width="104.7109375" customWidth="1"/>
+    <col min="16" max="16" width="56.7109375" customWidth="1"/>
+    <col min="17" max="17" width="64.7109375" customWidth="1"/>
     <col min="18" max="18" width="76.7109375" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="58.7109375" hidden="1" customWidth="1"/>
     <col min="20" max="20" width="54.7109375" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="12.7109375" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="16.7109375" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="12.7109375" customWidth="1"/>
+    <col min="22" max="22" width="16.7109375" customWidth="1"/>
     <col min="23" max="23" width="18.7109375" hidden="1" customWidth="1"/>
-    <col min="24" max="25" width="6.7109375" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="64.7109375" hidden="1" customWidth="1"/>
-    <col min="27" max="27" width="96.7109375" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="98.7109375" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="110.7109375" hidden="1" customWidth="1"/>
-    <col min="30" max="30" width="62.7109375" hidden="1" customWidth="1"/>
-    <col min="31" max="31" width="70.7109375" hidden="1" customWidth="1"/>
+    <col min="24" max="25" width="6.7109375" customWidth="1"/>
+    <col min="26" max="26" width="64.7109375" customWidth="1"/>
+    <col min="27" max="27" width="96.7109375" customWidth="1"/>
+    <col min="28" max="28" width="98.7109375" customWidth="1"/>
+    <col min="29" max="29" width="110.7109375" customWidth="1"/>
+    <col min="30" max="30" width="62.7109375" customWidth="1"/>
+    <col min="31" max="31" width="70.7109375" customWidth="1"/>
     <col min="32" max="32" width="82.7109375" hidden="1" customWidth="1"/>
     <col min="33" max="33" width="64.7109375" hidden="1" customWidth="1"/>
     <col min="34" max="34" width="60.7109375" hidden="1" customWidth="1"/>
-    <col min="35" max="35" width="58.7109375" hidden="1" customWidth="1"/>
-    <col min="36" max="36" width="66.7109375" hidden="1" customWidth="1"/>
+    <col min="35" max="35" width="58.7109375" customWidth="1"/>
+    <col min="36" max="36" width="66.7109375" customWidth="1"/>
     <col min="37" max="37" width="78.7109375" hidden="1" customWidth="1"/>
     <col min="38" max="38" width="60.7109375" hidden="1" customWidth="1"/>
     <col min="39" max="39" width="56.7109375" hidden="1" customWidth="1"/>
-    <col min="40" max="40" width="20.7109375" style="2" hidden="1" customWidth="1"/>
-    <col min="41" max="41" width="28.7109375" hidden="1" customWidth="1"/>
-    <col min="42" max="42" width="30.7109375" hidden="1" customWidth="1"/>
-    <col min="43" max="43" width="42.7109375" hidden="1" customWidth="1"/>
-    <col min="44" max="44" width="50.7109375" hidden="1" customWidth="1"/>
+    <col min="40" max="40" width="20.7109375" style="2" customWidth="1"/>
+    <col min="41" max="41" width="28.7109375" customWidth="1"/>
+    <col min="42" max="42" width="30.7109375" customWidth="1"/>
+    <col min="43" max="43" width="42.7109375" customWidth="1"/>
+    <col min="44" max="44" width="50.7109375" customWidth="1"/>
     <col min="45" max="45" width="62.7109375" hidden="1" customWidth="1"/>
     <col min="46" max="46" width="44.7109375" hidden="1" customWidth="1"/>
     <col min="47" max="47" width="40.7109375" hidden="1" customWidth="1"/>
-    <col min="48" max="48" width="30.7109375" style="2" hidden="1" customWidth="1"/>
-    <col min="49" max="49" width="16.7109375" hidden="1" customWidth="1"/>
-    <col min="50" max="50" width="26.7109375" hidden="1" customWidth="1"/>
-    <col min="51" max="51" width="44.7109375" style="2" hidden="1" customWidth="1"/>
-    <col min="52" max="52" width="42.7109375" hidden="1" customWidth="1"/>
-    <col min="53" max="53" width="48.7109375" hidden="1" customWidth="1"/>
-    <col min="54" max="54" width="40.7109375" hidden="1" customWidth="1"/>
-    <col min="55" max="55" width="30.7109375" hidden="1" customWidth="1"/>
-    <col min="56" max="56" width="40.7109375" hidden="1" customWidth="1"/>
-    <col min="57" max="57" width="34.7109375" hidden="1" customWidth="1"/>
+    <col min="48" max="48" width="30.7109375" style="2" customWidth="1"/>
+    <col min="49" max="49" width="16.7109375" customWidth="1"/>
+    <col min="50" max="50" width="26.7109375" customWidth="1"/>
+    <col min="51" max="51" width="44.7109375" style="2" customWidth="1"/>
+    <col min="52" max="52" width="42.7109375" customWidth="1"/>
+    <col min="53" max="53" width="48.7109375" customWidth="1"/>
+    <col min="54" max="54" width="40.7109375" customWidth="1"/>
+    <col min="55" max="55" width="30.7109375" customWidth="1"/>
+    <col min="56" max="56" width="40.7109375" customWidth="1"/>
+    <col min="57" max="57" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:57" hidden="1">
@@ -43859,52 +43860,52 @@
     <col min="14" max="14" width="116.7109375" customWidth="1"/>
     <col min="15" max="15" width="128.7109375" customWidth="1"/>
     <col min="16" max="16" width="78.7109375" customWidth="1"/>
-    <col min="17" max="17" width="28.7109375" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="32.7109375" hidden="1" customWidth="1"/>
-    <col min="19" max="20" width="20.7109375" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="14.7109375" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="28.7109375" customWidth="1"/>
+    <col min="18" max="18" width="32.7109375" customWidth="1"/>
+    <col min="19" max="20" width="20.7109375" customWidth="1"/>
+    <col min="21" max="21" width="14.7109375" customWidth="1"/>
     <col min="22" max="22" width="28.7109375" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="30.7109375" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="18.7109375" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="32.7109375" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="56.7109375" hidden="1" customWidth="1"/>
-    <col min="27" max="28" width="34.7109375" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="58.7109375" hidden="1" customWidth="1"/>
-    <col min="30" max="30" width="88.7109375" hidden="1" customWidth="1"/>
-    <col min="31" max="31" width="80.7109375" hidden="1" customWidth="1"/>
-    <col min="32" max="32" width="54.7109375" hidden="1" customWidth="1"/>
-    <col min="33" max="33" width="30.7109375" hidden="1" customWidth="1"/>
-    <col min="34" max="34" width="42.7109375" hidden="1" customWidth="1"/>
-    <col min="35" max="35" width="50.7109375" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="30.7109375" customWidth="1"/>
+    <col min="24" max="24" width="18.7109375" customWidth="1"/>
+    <col min="25" max="25" width="32.7109375" customWidth="1"/>
+    <col min="26" max="26" width="56.7109375" customWidth="1"/>
+    <col min="27" max="28" width="34.7109375" customWidth="1"/>
+    <col min="29" max="29" width="58.7109375" customWidth="1"/>
+    <col min="30" max="30" width="88.7109375" customWidth="1"/>
+    <col min="31" max="31" width="80.7109375" customWidth="1"/>
+    <col min="32" max="32" width="54.7109375" customWidth="1"/>
+    <col min="33" max="33" width="30.7109375" customWidth="1"/>
+    <col min="34" max="34" width="42.7109375" customWidth="1"/>
+    <col min="35" max="35" width="50.7109375" customWidth="1"/>
     <col min="36" max="36" width="62.7109375" hidden="1" customWidth="1"/>
     <col min="37" max="37" width="44.7109375" hidden="1" customWidth="1"/>
     <col min="38" max="38" width="40.7109375" hidden="1" customWidth="1"/>
-    <col min="39" max="39" width="30.7109375" style="2" hidden="1" customWidth="1"/>
-    <col min="40" max="40" width="16.7109375" hidden="1" customWidth="1"/>
-    <col min="41" max="41" width="44.7109375" hidden="1" customWidth="1"/>
-    <col min="42" max="42" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="43" max="44" width="20.7109375" hidden="1" customWidth="1"/>
-    <col min="45" max="45" width="22.7109375" style="2" hidden="1" customWidth="1"/>
-    <col min="46" max="46" width="12.7109375" hidden="1" customWidth="1"/>
-    <col min="47" max="48" width="66.7109375" hidden="1" customWidth="1"/>
-    <col min="49" max="49" width="58.7109375" hidden="1" customWidth="1"/>
-    <col min="50" max="50" width="72.7109375" hidden="1" customWidth="1"/>
-    <col min="51" max="51" width="76.7109375" hidden="1" customWidth="1"/>
-    <col min="52" max="52" width="126.7109375" hidden="1" customWidth="1"/>
-    <col min="53" max="53" width="118.7109375" hidden="1" customWidth="1"/>
-    <col min="54" max="54" width="122.7109375" hidden="1" customWidth="1"/>
-    <col min="55" max="55" width="114.7109375" hidden="1" customWidth="1"/>
-    <col min="56" max="56" width="102.7109375" hidden="1" customWidth="1"/>
-    <col min="57" max="57" width="126.7109375" hidden="1" customWidth="1"/>
-    <col min="58" max="59" width="104.7109375" hidden="1" customWidth="1"/>
-    <col min="60" max="60" width="88.7109375" hidden="1" customWidth="1"/>
-    <col min="61" max="61" width="92.7109375" hidden="1" customWidth="1"/>
-    <col min="62" max="62" width="38.7109375" hidden="1" customWidth="1"/>
-    <col min="63" max="63" width="46.7109375" hidden="1" customWidth="1"/>
+    <col min="39" max="39" width="30.7109375" style="2" customWidth="1"/>
+    <col min="40" max="40" width="16.7109375" customWidth="1"/>
+    <col min="41" max="41" width="44.7109375" customWidth="1"/>
+    <col min="42" max="42" width="36.7109375" customWidth="1"/>
+    <col min="43" max="44" width="20.7109375" customWidth="1"/>
+    <col min="45" max="45" width="22.7109375" style="2" customWidth="1"/>
+    <col min="46" max="46" width="12.7109375" customWidth="1"/>
+    <col min="47" max="48" width="66.7109375" customWidth="1"/>
+    <col min="49" max="49" width="58.7109375" customWidth="1"/>
+    <col min="50" max="50" width="72.7109375" customWidth="1"/>
+    <col min="51" max="51" width="76.7109375" customWidth="1"/>
+    <col min="52" max="52" width="126.7109375" customWidth="1"/>
+    <col min="53" max="53" width="118.7109375" customWidth="1"/>
+    <col min="54" max="54" width="122.7109375" customWidth="1"/>
+    <col min="55" max="55" width="114.7109375" customWidth="1"/>
+    <col min="56" max="56" width="102.7109375" customWidth="1"/>
+    <col min="57" max="57" width="126.7109375" customWidth="1"/>
+    <col min="58" max="59" width="104.7109375" customWidth="1"/>
+    <col min="60" max="60" width="88.7109375" customWidth="1"/>
+    <col min="61" max="61" width="92.7109375" customWidth="1"/>
+    <col min="62" max="62" width="38.7109375" customWidth="1"/>
+    <col min="63" max="63" width="46.7109375" customWidth="1"/>
     <col min="64" max="64" width="58.7109375" hidden="1" customWidth="1"/>
     <col min="65" max="65" width="40.7109375" hidden="1" customWidth="1"/>
     <col min="66" max="66" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="67" max="67" width="56.7109375" hidden="1" customWidth="1"/>
+    <col min="67" max="67" width="56.7109375" customWidth="1"/>
     <col min="68" max="68" width="88.7109375" hidden="1" customWidth="1"/>
     <col min="69" max="69" width="90.7109375" hidden="1" customWidth="1"/>
     <col min="70" max="70" width="102.7109375" hidden="1" customWidth="1"/>
@@ -44924,23 +44925,23 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="42.7109375" customWidth="1"/>
-    <col min="2" max="2" width="122.7109375" hidden="1" customWidth="1"/>
-    <col min="3" max="4" width="114.7109375" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="124.7109375" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="146.7109375" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="104.7109375" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="144.7109375" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="152.7109375" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="98.7109375" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="116.7109375" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="104.7109375" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="96.7109375" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="98.7109375" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="106.7109375" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="122.7109375" customWidth="1"/>
+    <col min="3" max="4" width="114.7109375" customWidth="1"/>
+    <col min="5" max="5" width="124.7109375" customWidth="1"/>
+    <col min="6" max="6" width="146.7109375" customWidth="1"/>
+    <col min="7" max="7" width="104.7109375" customWidth="1"/>
+    <col min="8" max="8" width="144.7109375" customWidth="1"/>
+    <col min="9" max="9" width="152.7109375" customWidth="1"/>
+    <col min="10" max="10" width="98.7109375" customWidth="1"/>
+    <col min="11" max="11" width="116.7109375" customWidth="1"/>
+    <col min="12" max="12" width="104.7109375" customWidth="1"/>
+    <col min="13" max="13" width="96.7109375" customWidth="1"/>
+    <col min="14" max="14" width="98.7109375" customWidth="1"/>
+    <col min="15" max="15" width="106.7109375" customWidth="1"/>
     <col min="16" max="16" width="118.7109375" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="100.7109375" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="96.7109375" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="116.7109375" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="116.7109375" customWidth="1"/>
     <col min="20" max="20" width="148.7109375" hidden="1" customWidth="1"/>
     <col min="21" max="21" width="150.7109375" hidden="1" customWidth="1"/>
     <col min="22" max="22" width="162.7109375" hidden="1" customWidth="1"/>
@@ -44949,32 +44950,32 @@
     <col min="25" max="25" width="134.7109375" hidden="1" customWidth="1"/>
     <col min="26" max="26" width="116.7109375" hidden="1" customWidth="1"/>
     <col min="27" max="27" width="112.7109375" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="90.7109375" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="102.7109375" hidden="1" customWidth="1"/>
-    <col min="30" max="30" width="110.7109375" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="90.7109375" customWidth="1"/>
+    <col min="29" max="29" width="102.7109375" customWidth="1"/>
+    <col min="30" max="30" width="110.7109375" customWidth="1"/>
     <col min="31" max="31" width="122.7109375" hidden="1" customWidth="1"/>
     <col min="32" max="32" width="104.7109375" hidden="1" customWidth="1"/>
     <col min="33" max="33" width="100.7109375" hidden="1" customWidth="1"/>
-    <col min="34" max="34" width="90.7109375" style="2" hidden="1" customWidth="1"/>
-    <col min="35" max="35" width="48.7109375" hidden="1" customWidth="1"/>
-    <col min="36" max="36" width="146.7109375" hidden="1" customWidth="1"/>
-    <col min="37" max="37" width="172.7109375" hidden="1" customWidth="1"/>
-    <col min="38" max="38" width="120.7109375" hidden="1" customWidth="1"/>
-    <col min="39" max="39" width="44.7109375" hidden="1" customWidth="1"/>
-    <col min="40" max="40" width="52.7109375" hidden="1" customWidth="1"/>
-    <col min="41" max="41" width="130.7109375" hidden="1" customWidth="1"/>
-    <col min="42" max="42" width="156.7109375" hidden="1" customWidth="1"/>
-    <col min="43" max="43" width="126.7109375" hidden="1" customWidth="1"/>
-    <col min="44" max="44" width="72.7109375" hidden="1" customWidth="1"/>
-    <col min="45" max="45" width="60.7109375" hidden="1" customWidth="1"/>
-    <col min="46" max="46" width="80.7109375" hidden="1" customWidth="1"/>
-    <col min="47" max="47" width="72.7109375" hidden="1" customWidth="1"/>
-    <col min="48" max="48" width="74.7109375" hidden="1" customWidth="1"/>
-    <col min="49" max="49" width="82.7109375" hidden="1" customWidth="1"/>
+    <col min="34" max="34" width="90.7109375" style="2" customWidth="1"/>
+    <col min="35" max="35" width="48.7109375" customWidth="1"/>
+    <col min="36" max="36" width="146.7109375" customWidth="1"/>
+    <col min="37" max="37" width="172.7109375" customWidth="1"/>
+    <col min="38" max="38" width="120.7109375" customWidth="1"/>
+    <col min="39" max="39" width="44.7109375" customWidth="1"/>
+    <col min="40" max="40" width="52.7109375" customWidth="1"/>
+    <col min="41" max="41" width="130.7109375" customWidth="1"/>
+    <col min="42" max="42" width="156.7109375" customWidth="1"/>
+    <col min="43" max="43" width="126.7109375" customWidth="1"/>
+    <col min="44" max="44" width="72.7109375" customWidth="1"/>
+    <col min="45" max="45" width="60.7109375" customWidth="1"/>
+    <col min="46" max="46" width="80.7109375" customWidth="1"/>
+    <col min="47" max="47" width="72.7109375" customWidth="1"/>
+    <col min="48" max="48" width="74.7109375" customWidth="1"/>
+    <col min="49" max="49" width="82.7109375" customWidth="1"/>
     <col min="50" max="50" width="94.7109375" hidden="1" customWidth="1"/>
     <col min="51" max="51" width="76.7109375" hidden="1" customWidth="1"/>
     <col min="52" max="52" width="72.7109375" hidden="1" customWidth="1"/>
-    <col min="53" max="53" width="92.7109375" hidden="1" customWidth="1"/>
+    <col min="53" max="53" width="92.7109375" customWidth="1"/>
     <col min="54" max="54" width="124.7109375" hidden="1" customWidth="1"/>
     <col min="55" max="55" width="126.7109375" hidden="1" customWidth="1"/>
     <col min="56" max="56" width="138.7109375" hidden="1" customWidth="1"/>
@@ -44983,23 +44984,23 @@
     <col min="59" max="59" width="110.7109375" hidden="1" customWidth="1"/>
     <col min="60" max="60" width="92.7109375" hidden="1" customWidth="1"/>
     <col min="61" max="61" width="88.7109375" hidden="1" customWidth="1"/>
-    <col min="62" max="62" width="66.7109375" hidden="1" customWidth="1"/>
-    <col min="63" max="63" width="78.7109375" hidden="1" customWidth="1"/>
-    <col min="64" max="64" width="86.7109375" hidden="1" customWidth="1"/>
+    <col min="62" max="62" width="66.7109375" customWidth="1"/>
+    <col min="63" max="63" width="78.7109375" customWidth="1"/>
+    <col min="64" max="64" width="86.7109375" customWidth="1"/>
     <col min="65" max="65" width="98.7109375" hidden="1" customWidth="1"/>
     <col min="66" max="66" width="80.7109375" hidden="1" customWidth="1"/>
     <col min="67" max="67" width="76.7109375" hidden="1" customWidth="1"/>
-    <col min="68" max="68" width="66.7109375" style="2" hidden="1" customWidth="1"/>
-    <col min="69" max="70" width="48.7109375" hidden="1" customWidth="1"/>
-    <col min="71" max="72" width="64.7109375" hidden="1" customWidth="1"/>
-    <col min="73" max="73" width="84.7109375" hidden="1" customWidth="1"/>
-    <col min="74" max="74" width="76.7109375" hidden="1" customWidth="1"/>
-    <col min="75" max="75" width="78.7109375" hidden="1" customWidth="1"/>
-    <col min="76" max="76" width="86.7109375" hidden="1" customWidth="1"/>
+    <col min="68" max="68" width="66.7109375" style="2" customWidth="1"/>
+    <col min="69" max="70" width="48.7109375" customWidth="1"/>
+    <col min="71" max="72" width="64.7109375" customWidth="1"/>
+    <col min="73" max="73" width="84.7109375" customWidth="1"/>
+    <col min="74" max="74" width="76.7109375" customWidth="1"/>
+    <col min="75" max="75" width="78.7109375" customWidth="1"/>
+    <col min="76" max="76" width="86.7109375" customWidth="1"/>
     <col min="77" max="77" width="98.7109375" hidden="1" customWidth="1"/>
     <col min="78" max="78" width="80.7109375" hidden="1" customWidth="1"/>
     <col min="79" max="79" width="76.7109375" hidden="1" customWidth="1"/>
-    <col min="80" max="80" width="96.7109375" hidden="1" customWidth="1"/>
+    <col min="80" max="80" width="96.7109375" customWidth="1"/>
     <col min="81" max="81" width="128.7109375" hidden="1" customWidth="1"/>
     <col min="82" max="82" width="130.7109375" hidden="1" customWidth="1"/>
     <col min="83" max="83" width="142.7109375" hidden="1" customWidth="1"/>
@@ -45008,13 +45009,13 @@
     <col min="86" max="86" width="114.7109375" hidden="1" customWidth="1"/>
     <col min="87" max="87" width="96.7109375" hidden="1" customWidth="1"/>
     <col min="88" max="88" width="92.7109375" hidden="1" customWidth="1"/>
-    <col min="89" max="89" width="70.7109375" hidden="1" customWidth="1"/>
-    <col min="90" max="90" width="82.7109375" hidden="1" customWidth="1"/>
-    <col min="91" max="91" width="90.7109375" hidden="1" customWidth="1"/>
+    <col min="89" max="89" width="70.7109375" customWidth="1"/>
+    <col min="90" max="90" width="82.7109375" customWidth="1"/>
+    <col min="91" max="91" width="90.7109375" customWidth="1"/>
     <col min="92" max="92" width="102.7109375" hidden="1" customWidth="1"/>
     <col min="93" max="93" width="84.7109375" hidden="1" customWidth="1"/>
     <col min="94" max="94" width="80.7109375" hidden="1" customWidth="1"/>
-    <col min="95" max="95" width="70.7109375" style="2" hidden="1" customWidth="1"/>
+    <col min="95" max="95" width="70.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:95" hidden="1">
@@ -46376,8 +46377,8 @@
   <cols>
     <col min="1" max="1" width="26.7109375" customWidth="1"/>
     <col min="2" max="2" width="48.7109375" customWidth="1"/>
-    <col min="3" max="3" width="62.7109375" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="54.7109375" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="62.7109375" customWidth="1"/>
+    <col min="4" max="4" width="54.7109375" customWidth="1"/>
     <col min="5" max="5" width="56.7109375" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="64.7109375" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="76.7109375" hidden="1" customWidth="1"/>
@@ -46392,32 +46393,32 @@
     <col min="16" max="16" width="92.7109375" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="74.7109375" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="70.7109375" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="48.7109375" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="60.7109375" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="68.7109375" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="48.7109375" customWidth="1"/>
+    <col min="20" max="20" width="60.7109375" customWidth="1"/>
+    <col min="21" max="21" width="68.7109375" customWidth="1"/>
     <col min="22" max="22" width="80.7109375" hidden="1" customWidth="1"/>
     <col min="23" max="23" width="62.7109375" hidden="1" customWidth="1"/>
     <col min="24" max="24" width="58.7109375" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="48.7109375" style="2" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="48.7109375" style="2" customWidth="1"/>
     <col min="26" max="26" width="42.7109375" customWidth="1"/>
-    <col min="27" max="27" width="38.7109375" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="50.7109375" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="64.7109375" hidden="1" customWidth="1"/>
-    <col min="30" max="30" width="80.7109375" hidden="1" customWidth="1"/>
-    <col min="31" max="31" width="38.7109375" hidden="1" customWidth="1"/>
-    <col min="32" max="32" width="74.7109375" hidden="1" customWidth="1"/>
-    <col min="33" max="33" width="66.7109375" hidden="1" customWidth="1"/>
-    <col min="34" max="37" width="52.7109375" hidden="1" customWidth="1"/>
-    <col min="38" max="38" width="66.7109375" hidden="1" customWidth="1"/>
-    <col min="39" max="39" width="68.7109375" hidden="1" customWidth="1"/>
-    <col min="40" max="40" width="66.7109375" hidden="1" customWidth="1"/>
-    <col min="41" max="41" width="60.7109375" hidden="1" customWidth="1"/>
-    <col min="42" max="42" width="72.7109375" hidden="1" customWidth="1"/>
-    <col min="43" max="43" width="80.7109375" hidden="1" customWidth="1"/>
+    <col min="27" max="27" width="38.7109375" customWidth="1"/>
+    <col min="28" max="28" width="50.7109375" customWidth="1"/>
+    <col min="29" max="29" width="64.7109375" customWidth="1"/>
+    <col min="30" max="30" width="80.7109375" customWidth="1"/>
+    <col min="31" max="31" width="38.7109375" customWidth="1"/>
+    <col min="32" max="32" width="74.7109375" customWidth="1"/>
+    <col min="33" max="33" width="66.7109375" customWidth="1"/>
+    <col min="34" max="37" width="52.7109375" customWidth="1"/>
+    <col min="38" max="38" width="66.7109375" customWidth="1"/>
+    <col min="39" max="39" width="68.7109375" customWidth="1"/>
+    <col min="40" max="40" width="66.7109375" customWidth="1"/>
+    <col min="41" max="41" width="60.7109375" customWidth="1"/>
+    <col min="42" max="42" width="72.7109375" customWidth="1"/>
+    <col min="43" max="43" width="80.7109375" customWidth="1"/>
     <col min="44" max="44" width="92.7109375" hidden="1" customWidth="1"/>
     <col min="45" max="45" width="74.7109375" hidden="1" customWidth="1"/>
     <col min="46" max="46" width="70.7109375" hidden="1" customWidth="1"/>
-    <col min="47" max="47" width="60.7109375" style="2" hidden="1" customWidth="1"/>
+    <col min="47" max="47" width="60.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:47" hidden="1">

</xml_diff>

<commit_message>
Added new source for xsd schema
</commit_message>
<xml_diff>
--- a/data/bodem_template.xlsx
+++ b/data/bodem_template.xlsx
@@ -47187,7 +47187,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.7109375" customWidth="1"/>
-    <col min="2" max="2" width="54.7109375" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="86.7109375" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="88.7109375" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="100.7109375" hidden="1" customWidth="1"/>
@@ -47196,7 +47196,7 @@
     <col min="8" max="8" width="72.7109375" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="54.7109375" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="50.7109375" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="54.7109375" customWidth="1"/>
+    <col min="11" max="11" width="26.7109375" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="86.7109375" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="88.7109375" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="100.7109375" hidden="1" customWidth="1"/>
@@ -47208,7 +47208,7 @@
     <col min="20" max="20" width="44.7109375" hidden="1" customWidth="1"/>
     <col min="21" max="21" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="22" max="22" width="24.7109375" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="58.7109375" customWidth="1"/>
+    <col min="23" max="23" width="30.7109375" hidden="1" customWidth="1"/>
     <col min="24" max="24" width="90.7109375" hidden="1" customWidth="1"/>
     <col min="25" max="25" width="92.7109375" hidden="1" customWidth="1"/>
     <col min="26" max="26" width="104.7109375" hidden="1" customWidth="1"/>

</xml_diff>

<commit_message>
Fixed encoding problem with config file
</commit_message>
<xml_diff>
--- a/data/bodem_template.xlsx
+++ b/data/bodem_template.xlsx
@@ -335,13 +335,13 @@
     <t>CHEM_FYS</t>
   </si>
   <si>
-    <t>x-coÃ¶rdinaat beginpunt</t>
-  </si>
-  <si>
-    <t>y-coÃ¶rdinaat beginpunt</t>
-  </si>
-  <si>
-    <t>methode opmeten xy-coÃ¶rdinaten beginpunt</t>
+    <t>x-coördinaat beginpunt</t>
+  </si>
+  <si>
+    <t>y-coördinaat beginpunt</t>
+  </si>
+  <si>
+    <t>methode opmeten xy-coördinaten beginpunt</t>
   </si>
   <si>
     <t>gedigitaliseerd in Google Earth</t>
@@ -386,10 +386,10 @@
     <t>getransformeerde coördinaten uit dossier</t>
   </si>
   <si>
-    <t>naam opmeten xy-coÃ¶rdinaten beginpunt</t>
-  </si>
-  <si>
-    <t>betrouwbaarheid xy-coÃ¶rdinaten beginpunt</t>
+    <t>naam opmeten xy-coördinaten beginpunt</t>
+  </si>
+  <si>
+    <t>betrouwbaarheid xy-coördinaten beginpunt</t>
   </si>
   <si>
     <t>goed</t>
@@ -449,19 +449,19 @@
     <t>betrouwbaarheid maaiveld beginpunt</t>
   </si>
   <si>
-    <t>x-coÃ¶rdinaat eindpunt</t>
-  </si>
-  <si>
-    <t>y-coÃ¶rdinaat eindpunt</t>
-  </si>
-  <si>
-    <t>betrouwbaarheid xy-coÃ¶rdinaten eindpunt</t>
-  </si>
-  <si>
-    <t>methode opmeten xy-coÃ¶rdinaten eindpunt</t>
-  </si>
-  <si>
-    <t>naam opmeten xy-coÃ¶rdinaten eindpunt</t>
+    <t>x-coördinaat eindpunt</t>
+  </si>
+  <si>
+    <t>y-coördinaat eindpunt</t>
+  </si>
+  <si>
+    <t>betrouwbaarheid xy-coördinaten eindpunt</t>
+  </si>
+  <si>
+    <t>methode opmeten xy-coördinaten eindpunt</t>
+  </si>
+  <si>
+    <t>naam opmeten xy-coördinaten eindpunt</t>
   </si>
   <si>
     <t>waarde maaiveld eindpunt (mTAW)</t>
@@ -731,7 +731,7 @@
     <t>geometrie</t>
   </si>
   <si>
-    <t>geometrie coÃ¶rdinatenstelsel</t>
+    <t>geometrie coördinatenstelsel</t>
   </si>
   <si>
     <t>geometrie wkt</t>
@@ -4871,7 +4871,7 @@
     <t>Date generated</t>
   </si>
   <si>
-    <t>2024-07-24 08:44:24.116187</t>
+    <t>2024-07-24 09:00:00.647555</t>
   </si>
   <si>
     <t>version</t>
@@ -34991,17 +34991,17 @@
   <cols>
     <col min="1" max="3" width="8.7109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="32.7109375" style="3" customWidth="1"/>
-    <col min="5" max="6" width="46.7109375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="82.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="76.7109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="82.7109375" style="2" customWidth="1"/>
+    <col min="5" max="6" width="44.7109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="80.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="74.7109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="80.7109375" style="2" customWidth="1"/>
     <col min="10" max="10" width="64.7109375" style="4" customWidth="1"/>
     <col min="11" max="11" width="68.7109375" style="2" customWidth="1"/>
     <col min="12" max="12" width="62.7109375" style="2" customWidth="1"/>
     <col min="13" max="13" width="68.7109375" style="2" customWidth="1"/>
-    <col min="14" max="15" width="44.7109375" style="4" customWidth="1"/>
-    <col min="16" max="17" width="80.7109375" style="2" customWidth="1"/>
-    <col min="18" max="18" width="74.7109375" style="2" customWidth="1"/>
+    <col min="14" max="15" width="42.7109375" style="4" customWidth="1"/>
+    <col min="16" max="17" width="78.7109375" style="2" customWidth="1"/>
+    <col min="18" max="18" width="72.7109375" style="2" customWidth="1"/>
     <col min="19" max="19" width="62.7109375" style="4" customWidth="1"/>
     <col min="20" max="21" width="66.7109375" style="2" customWidth="1"/>
     <col min="22" max="22" width="60.7109375" style="2" customWidth="1"/>
@@ -35700,12 +35700,12 @@
   <hyperlinks>
     <hyperlink ref="B8" location="'Codelijsten'!$A$2" display="type"/>
     <hyperlink ref="C8" location="'Codelijsten'!$C$2" display="doel"/>
-    <hyperlink ref="G8" location="'Codelijsten'!$E$2" display="methode opmeten xy-coÃ¶rdinaten beginpunt"/>
-    <hyperlink ref="I8" location="'Codelijsten'!$G$2" display="betrouwbaarheid xy-coÃ¶rdinaten beginpunt"/>
+    <hyperlink ref="G8" location="'Codelijsten'!$E$2" display="methode opmeten xy-coördinaten beginpunt"/>
+    <hyperlink ref="I8" location="'Codelijsten'!$G$2" display="betrouwbaarheid xy-coördinaten beginpunt"/>
     <hyperlink ref="K8" location="'Codelijsten'!$I$2" display="methode opmeten maaiveld beginpunt"/>
     <hyperlink ref="M8" location="'Codelijsten'!$K$2" display="betrouwbaarheid maaiveld beginpunt"/>
-    <hyperlink ref="P8" location="'Codelijsten'!$M$2" display="betrouwbaarheid xy-coÃ¶rdinaten eindpunt"/>
-    <hyperlink ref="Q8" location="'Codelijsten'!$O$2" display="methode opmeten xy-coÃ¶rdinaten eindpunt"/>
+    <hyperlink ref="P8" location="'Codelijsten'!$M$2" display="betrouwbaarheid xy-coördinaten eindpunt"/>
+    <hyperlink ref="Q8" location="'Codelijsten'!$O$2" display="methode opmeten xy-coördinaten eindpunt"/>
     <hyperlink ref="T8" location="'Codelijsten'!$Q$2" display="betrouwbaarheid maaiveld eindpunt"/>
     <hyperlink ref="U8" location="'Codelijsten'!$S$2" display="methode opmeten maaiveld eindpunt"/>
     <hyperlink ref="AE8" location="'Codelijsten'!$U$2" display="status"/>
@@ -35726,7 +35726,7 @@
     <col min="1" max="1" width="8.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="24.7109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="32.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="58.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="56.7109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="26.7109375" style="2" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" style="2" customWidth="1"/>
     <col min="7" max="7" width="22.7109375" style="2" hidden="1" customWidth="1"/>

</xml_diff>

<commit_message>
Updated config files for opdracht
</commit_message>
<xml_diff>
--- a/data/bodem_template.xlsx
+++ b/data/bodem_template.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9901" uniqueCount="1621">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9959" uniqueCount="1648">
   <si>
     <t>naam</t>
   </si>
@@ -4805,12 +4805,30 @@
     <t>dataleverancier-choice_1-naam</t>
   </si>
   <si>
+    <t>kwaliteit-aard</t>
+  </si>
+  <si>
+    <t>aard</t>
+  </si>
+  <si>
+    <t>kwaliteit-origine</t>
+  </si>
+  <si>
+    <t>origine</t>
+  </si>
+  <si>
+    <t>kwaliteit</t>
+  </si>
+  <si>
     <t>startdatum</t>
   </si>
   <si>
     <t>einddatum</t>
   </si>
   <si>
+    <t>omschrijving</t>
+  </si>
+  <si>
     <t>locatie-coordinatenstelsel</t>
   </si>
   <si>
@@ -4820,13 +4838,76 @@
     <t>locatie</t>
   </si>
   <si>
-    <t>kwaliteit-origine</t>
-  </si>
-  <si>
-    <t>origine</t>
-  </si>
-  <si>
-    <t>kwaliteit</t>
+    <t>Geologisch onderzoek</t>
+  </si>
+  <si>
+    <t>Exploratie minerale bronnen</t>
+  </si>
+  <si>
+    <t>Exploitatie minerale bronnen</t>
+  </si>
+  <si>
+    <t>Exploratie energie bronnen</t>
+  </si>
+  <si>
+    <t>Exploitatie energie bronnen</t>
+  </si>
+  <si>
+    <t>Geothermie</t>
+  </si>
+  <si>
+    <t>Berging</t>
+  </si>
+  <si>
+    <t>Exploratie ondergrondse opslag</t>
+  </si>
+  <si>
+    <t>Grondwaterwinning</t>
+  </si>
+  <si>
+    <t>Geofysisch onderzoek</t>
+  </si>
+  <si>
+    <t>Hydrogeologisch onderzoek</t>
+  </si>
+  <si>
+    <t>Bodemkundig onderzoek</t>
+  </si>
+  <si>
+    <t>Geotechnisch onderzoek</t>
+  </si>
+  <si>
+    <t>Geochemisch onderzoek</t>
+  </si>
+  <si>
+    <t>Grondwaterkwaliteit monitoring</t>
+  </si>
+  <si>
+    <t>Grondwaterkwantiteit monitoring</t>
+  </si>
+  <si>
+    <t>Monitoring vervuilde sites</t>
+  </si>
+  <si>
+    <t>Drainage en bemaling</t>
+  </si>
+  <si>
+    <t>Sanering</t>
+  </si>
+  <si>
+    <t>Infiltratie</t>
+  </si>
+  <si>
+    <t>Meerdere</t>
+  </si>
+  <si>
+    <t>Bodemchemisch en bodemfysisch onderzoek</t>
+  </si>
+  <si>
+    <t>PFAS onderzoek</t>
+  </si>
+  <si>
+    <t>CTE onderzoek</t>
   </si>
   <si>
     <t>VLAREM</t>
@@ -4871,7 +4952,7 @@
     <t>Date generated</t>
   </si>
   <si>
-    <t>2024-07-24 09:00:00.647555</t>
+    <t>2024-07-24 13:26:29.895029</t>
   </si>
   <si>
     <t>version</t>
@@ -5305,7 +5386,7 @@
 </file>
 
 <file path=xl/tables/table39.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="39" name="Table39" displayName="Table39" ref="BY3:BZ8" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="39" name="Table39" displayName="Table39" ref="BY3:BZ27" totalsRowShown="0">
   <tableColumns count="2">
     <tableColumn id="1" name="Code"/>
     <tableColumn id="2" name="Beschrijving"/>
@@ -5335,7 +5416,17 @@
 </file>
 
 <file path=xl/tables/table41.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="41" name="Table41" displayName="Table41" ref="CC3:CD60" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="41" name="Table41" displayName="Table41" ref="CC3:CD8" totalsRowShown="0">
+  <tableColumns count="2">
+    <tableColumn id="1" name="Code"/>
+    <tableColumn id="2" name="Beschrijving"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table42.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="42" name="Table42" displayName="Table42" ref="CE3:CF60" totalsRowShown="0">
   <tableColumns count="2">
     <tableColumn id="1" name="Code"/>
     <tableColumn id="2" name="Beschrijving"/>
@@ -5679,16 +5770,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CD921"/>
+  <dimension ref="A1:CF921"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="83" width="10.7109375" customWidth="1"/>
+    <col min="1" max="85" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:82">
+    <row r="1" spans="1:84">
       <c r="A1" s="1" t="s">
         <v>230</v>
       </c>
@@ -5783,8 +5874,10 @@
       <c r="CB1" s="1"/>
       <c r="CC1" s="1"/>
       <c r="CD1" s="1"/>
-    </row>
-    <row r="2" spans="1:82">
+      <c r="CE1" s="1"/>
+      <c r="CF1" s="1"/>
+    </row>
+    <row r="2" spans="1:84">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -5938,19 +6031,23 @@
       </c>
       <c r="BX2" s="1"/>
       <c r="BY2" s="1" t="s">
-        <v>50</v>
+        <v>1595</v>
       </c>
       <c r="BZ2" s="1"/>
       <c r="CA2" s="1" t="s">
-        <v>1599</v>
+        <v>1597</v>
       </c>
       <c r="CB2" s="1"/>
       <c r="CC2" s="1" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="CD2" s="1"/>
-    </row>
-    <row r="3" spans="1:82">
+      <c r="CE2" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="CF2" s="1"/>
+    </row>
+    <row r="3" spans="1:84">
       <c r="A3" t="s">
         <v>84</v>
       </c>
@@ -6197,8 +6294,14 @@
       <c r="CD3" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="4" spans="1:82">
+      <c r="CE3" t="s">
+        <v>84</v>
+      </c>
+      <c r="CF3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:84">
       <c r="A4" t="s">
         <v>81</v>
       </c>
@@ -6428,25 +6531,31 @@
         <v>82</v>
       </c>
       <c r="BY4" t="s">
+        <v>1605</v>
+      </c>
+      <c r="BZ4" t="s">
+        <v>82</v>
+      </c>
+      <c r="CA4" t="s">
+        <v>1629</v>
+      </c>
+      <c r="CB4" t="s">
+        <v>82</v>
+      </c>
+      <c r="CC4" t="s">
         <v>156</v>
       </c>
-      <c r="BZ4" t="s">
-        <v>82</v>
-      </c>
-      <c r="CA4" t="s">
-        <v>1602</v>
-      </c>
-      <c r="CB4" t="s">
-        <v>82</v>
-      </c>
-      <c r="CC4" t="s">
+      <c r="CD4" t="s">
+        <v>82</v>
+      </c>
+      <c r="CE4" t="s">
         <v>171</v>
       </c>
-      <c r="CD4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:82">
+      <c r="CF4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:84">
       <c r="A5" t="s">
         <v>83</v>
       </c>
@@ -6676,25 +6785,31 @@
         <v>82</v>
       </c>
       <c r="BY5" t="s">
+        <v>1606</v>
+      </c>
+      <c r="BZ5" t="s">
+        <v>82</v>
+      </c>
+      <c r="CA5" t="s">
+        <v>1630</v>
+      </c>
+      <c r="CB5" t="s">
+        <v>82</v>
+      </c>
+      <c r="CC5" t="s">
         <v>157</v>
       </c>
-      <c r="BZ5" t="s">
-        <v>82</v>
-      </c>
-      <c r="CA5" t="s">
-        <v>1603</v>
-      </c>
-      <c r="CB5" t="s">
-        <v>82</v>
-      </c>
-      <c r="CC5" t="s">
+      <c r="CD5" t="s">
+        <v>82</v>
+      </c>
+      <c r="CE5" t="s">
         <v>172</v>
       </c>
-      <c r="CD5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:82">
+      <c r="CF5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:84">
       <c r="C6" t="s">
         <v>88</v>
       </c>
@@ -6900,25 +7015,31 @@
         <v>82</v>
       </c>
       <c r="BY6" t="s">
+        <v>1607</v>
+      </c>
+      <c r="BZ6" t="s">
+        <v>82</v>
+      </c>
+      <c r="CA6" t="s">
+        <v>1631</v>
+      </c>
+      <c r="CB6" t="s">
+        <v>82</v>
+      </c>
+      <c r="CC6" t="s">
         <v>158</v>
       </c>
-      <c r="BZ6" t="s">
-        <v>82</v>
-      </c>
-      <c r="CA6" t="s">
-        <v>1604</v>
-      </c>
-      <c r="CB6" t="s">
-        <v>82</v>
-      </c>
-      <c r="CC6" t="s">
+      <c r="CD6" t="s">
+        <v>82</v>
+      </c>
+      <c r="CE6" t="s">
         <v>173</v>
       </c>
-      <c r="CD6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="1:82">
+      <c r="CF6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:84">
       <c r="C7" t="s">
         <v>89</v>
       </c>
@@ -7058,25 +7179,31 @@
         <v>82</v>
       </c>
       <c r="BY7" t="s">
+        <v>1608</v>
+      </c>
+      <c r="BZ7" t="s">
+        <v>82</v>
+      </c>
+      <c r="CA7" t="s">
+        <v>1632</v>
+      </c>
+      <c r="CB7" t="s">
+        <v>82</v>
+      </c>
+      <c r="CC7" t="s">
         <v>159</v>
       </c>
-      <c r="BZ7" t="s">
-        <v>82</v>
-      </c>
-      <c r="CA7" t="s">
-        <v>1605</v>
-      </c>
-      <c r="CB7" t="s">
-        <v>82</v>
-      </c>
-      <c r="CC7" t="s">
+      <c r="CD7" t="s">
+        <v>82</v>
+      </c>
+      <c r="CE7" t="s">
         <v>174</v>
       </c>
-      <c r="CD7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:82">
+      <c r="CF7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:84">
       <c r="C8" t="s">
         <v>90</v>
       </c>
@@ -7210,25 +7337,31 @@
         <v>82</v>
       </c>
       <c r="BY8" t="s">
+        <v>1609</v>
+      </c>
+      <c r="BZ8" t="s">
+        <v>82</v>
+      </c>
+      <c r="CA8" t="s">
+        <v>1633</v>
+      </c>
+      <c r="CB8" t="s">
+        <v>82</v>
+      </c>
+      <c r="CC8" t="s">
         <v>160</v>
       </c>
-      <c r="BZ8" t="s">
-        <v>82</v>
-      </c>
-      <c r="CA8" t="s">
-        <v>1606</v>
-      </c>
-      <c r="CB8" t="s">
-        <v>82</v>
-      </c>
-      <c r="CC8" t="s">
+      <c r="CD8" t="s">
+        <v>82</v>
+      </c>
+      <c r="CE8" t="s">
         <v>175</v>
       </c>
-      <c r="CD8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9" spans="1:82">
+      <c r="CF8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:84">
       <c r="C9" t="s">
         <v>91</v>
       </c>
@@ -7337,20 +7470,26 @@
       <c r="BV9" t="s">
         <v>82</v>
       </c>
+      <c r="BY9" t="s">
+        <v>1610</v>
+      </c>
+      <c r="BZ9" t="s">
+        <v>82</v>
+      </c>
       <c r="CA9" t="s">
-        <v>1607</v>
+        <v>1634</v>
       </c>
       <c r="CB9" t="s">
         <v>82</v>
       </c>
-      <c r="CC9" t="s">
+      <c r="CE9" t="s">
         <v>176</v>
       </c>
-      <c r="CD9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:82">
+      <c r="CF9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:84">
       <c r="C10" t="s">
         <v>92</v>
       </c>
@@ -7453,20 +7592,26 @@
       <c r="BH10" t="s">
         <v>82</v>
       </c>
+      <c r="BY10" t="s">
+        <v>1611</v>
+      </c>
+      <c r="BZ10" t="s">
+        <v>82</v>
+      </c>
       <c r="CA10" t="s">
-        <v>1608</v>
+        <v>1635</v>
       </c>
       <c r="CB10" t="s">
         <v>82</v>
       </c>
-      <c r="CC10" t="s">
+      <c r="CE10" t="s">
         <v>177</v>
       </c>
-      <c r="CD10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="11" spans="1:82">
+      <c r="CF10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:84">
       <c r="C11" t="s">
         <v>93</v>
       </c>
@@ -7569,20 +7714,26 @@
       <c r="BH11" t="s">
         <v>82</v>
       </c>
+      <c r="BY11" t="s">
+        <v>1612</v>
+      </c>
+      <c r="BZ11" t="s">
+        <v>82</v>
+      </c>
       <c r="CA11" t="s">
-        <v>1609</v>
+        <v>1636</v>
       </c>
       <c r="CB11" t="s">
         <v>82</v>
       </c>
-      <c r="CC11" t="s">
+      <c r="CE11" t="s">
         <v>178</v>
       </c>
-      <c r="CD11" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="12" spans="1:82">
+      <c r="CF11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:84">
       <c r="C12" t="s">
         <v>94</v>
       </c>
@@ -7685,20 +7836,26 @@
       <c r="BH12" t="s">
         <v>82</v>
       </c>
+      <c r="BY12" t="s">
+        <v>1613</v>
+      </c>
+      <c r="BZ12" t="s">
+        <v>82</v>
+      </c>
       <c r="CA12" t="s">
-        <v>1610</v>
+        <v>1637</v>
       </c>
       <c r="CB12" t="s">
         <v>82</v>
       </c>
-      <c r="CC12" t="s">
+      <c r="CE12" t="s">
         <v>179</v>
       </c>
-      <c r="CD12" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:82">
+      <c r="CF12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:84">
       <c r="C13" t="s">
         <v>95</v>
       </c>
@@ -7801,20 +7958,26 @@
       <c r="BH13" t="s">
         <v>82</v>
       </c>
+      <c r="BY13" t="s">
+        <v>1614</v>
+      </c>
+      <c r="BZ13" t="s">
+        <v>82</v>
+      </c>
       <c r="CA13" t="s">
-        <v>1611</v>
+        <v>1638</v>
       </c>
       <c r="CB13" t="s">
         <v>82</v>
       </c>
-      <c r="CC13" t="s">
+      <c r="CE13" t="s">
         <v>180</v>
       </c>
-      <c r="CD13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:82">
+      <c r="CF13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:84">
       <c r="C14" t="s">
         <v>96</v>
       </c>
@@ -7917,20 +8080,26 @@
       <c r="BH14" t="s">
         <v>82</v>
       </c>
+      <c r="BY14" t="s">
+        <v>1615</v>
+      </c>
+      <c r="BZ14" t="s">
+        <v>82</v>
+      </c>
       <c r="CA14" t="s">
-        <v>1612</v>
+        <v>1639</v>
       </c>
       <c r="CB14" t="s">
         <v>82</v>
       </c>
-      <c r="CC14" t="s">
+      <c r="CE14" t="s">
         <v>181</v>
       </c>
-      <c r="CD14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" spans="1:82">
+      <c r="CF14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:84">
       <c r="C15" t="s">
         <v>97</v>
       </c>
@@ -8033,20 +8202,26 @@
       <c r="BH15" t="s">
         <v>82</v>
       </c>
+      <c r="BY15" t="s">
+        <v>1616</v>
+      </c>
+      <c r="BZ15" t="s">
+        <v>82</v>
+      </c>
       <c r="CA15" t="s">
-        <v>1613</v>
+        <v>1640</v>
       </c>
       <c r="CB15" t="s">
         <v>82</v>
       </c>
-      <c r="CC15" t="s">
+      <c r="CE15" t="s">
         <v>182</v>
       </c>
-      <c r="CD15" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="16" spans="1:82">
+      <c r="CF15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:84">
       <c r="C16" t="s">
         <v>98</v>
       </c>
@@ -8149,20 +8324,26 @@
       <c r="BH16" t="s">
         <v>82</v>
       </c>
+      <c r="BY16" t="s">
+        <v>1617</v>
+      </c>
+      <c r="BZ16" t="s">
+        <v>82</v>
+      </c>
       <c r="CA16" t="s">
-        <v>1614</v>
+        <v>1641</v>
       </c>
       <c r="CB16" t="s">
         <v>82</v>
       </c>
-      <c r="CC16" t="s">
+      <c r="CE16" t="s">
         <v>183</v>
       </c>
-      <c r="CD16" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="3:82">
+      <c r="CF16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="3:84">
       <c r="C17" t="s">
         <v>99</v>
       </c>
@@ -8265,20 +8446,26 @@
       <c r="BH17" t="s">
         <v>82</v>
       </c>
+      <c r="BY17" t="s">
+        <v>1618</v>
+      </c>
+      <c r="BZ17" t="s">
+        <v>82</v>
+      </c>
       <c r="CA17" t="s">
         <v>173</v>
       </c>
       <c r="CB17" t="s">
         <v>82</v>
       </c>
-      <c r="CC17" t="s">
+      <c r="CE17" t="s">
         <v>184</v>
       </c>
-      <c r="CD17" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="18" spans="3:82">
+      <c r="CF17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="3:84">
       <c r="C18" t="s">
         <v>100</v>
       </c>
@@ -8369,14 +8556,20 @@
       <c r="BH18" t="s">
         <v>82</v>
       </c>
-      <c r="CC18" t="s">
+      <c r="BY18" t="s">
+        <v>1619</v>
+      </c>
+      <c r="BZ18" t="s">
+        <v>82</v>
+      </c>
+      <c r="CE18" t="s">
         <v>185</v>
       </c>
-      <c r="CD18" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="19" spans="3:82">
+      <c r="CF18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="3:84">
       <c r="C19" t="s">
         <v>101</v>
       </c>
@@ -8467,14 +8660,20 @@
       <c r="BH19" t="s">
         <v>82</v>
       </c>
-      <c r="CC19" t="s">
+      <c r="BY19" t="s">
+        <v>1620</v>
+      </c>
+      <c r="BZ19" t="s">
+        <v>82</v>
+      </c>
+      <c r="CE19" t="s">
         <v>186</v>
       </c>
-      <c r="CD19" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="20" spans="3:82">
+      <c r="CF19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="3:84">
       <c r="C20" t="s">
         <v>102</v>
       </c>
@@ -8565,14 +8764,20 @@
       <c r="BH20" t="s">
         <v>82</v>
       </c>
-      <c r="CC20" t="s">
+      <c r="BY20" t="s">
+        <v>1621</v>
+      </c>
+      <c r="BZ20" t="s">
+        <v>82</v>
+      </c>
+      <c r="CE20" t="s">
         <v>187</v>
       </c>
-      <c r="CD20" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="21" spans="3:82">
+      <c r="CF20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="3:84">
       <c r="C21" t="s">
         <v>103</v>
       </c>
@@ -8651,14 +8856,20 @@
       <c r="BH21" t="s">
         <v>82</v>
       </c>
-      <c r="CC21" t="s">
+      <c r="BY21" t="s">
+        <v>1622</v>
+      </c>
+      <c r="BZ21" t="s">
+        <v>82</v>
+      </c>
+      <c r="CE21" t="s">
         <v>188</v>
       </c>
-      <c r="CD21" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="22" spans="3:82">
+      <c r="CF21" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="3:84">
       <c r="W22" t="s">
         <v>189</v>
       </c>
@@ -8731,14 +8942,20 @@
       <c r="BH22" t="s">
         <v>82</v>
       </c>
-      <c r="CC22" t="s">
+      <c r="BY22" t="s">
+        <v>1623</v>
+      </c>
+      <c r="BZ22" t="s">
+        <v>82</v>
+      </c>
+      <c r="CE22" t="s">
         <v>189</v>
       </c>
-      <c r="CD22" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="23" spans="3:82">
+      <c r="CF22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="3:84">
       <c r="W23" t="s">
         <v>190</v>
       </c>
@@ -8811,14 +9028,20 @@
       <c r="BH23" t="s">
         <v>82</v>
       </c>
-      <c r="CC23" t="s">
+      <c r="BY23" t="s">
+        <v>1624</v>
+      </c>
+      <c r="BZ23" t="s">
+        <v>82</v>
+      </c>
+      <c r="CE23" t="s">
         <v>190</v>
       </c>
-      <c r="CD23" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="24" spans="3:82">
+      <c r="CF23" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="3:84">
       <c r="W24" t="s">
         <v>191</v>
       </c>
@@ -8891,14 +9114,20 @@
       <c r="BH24" t="s">
         <v>82</v>
       </c>
-      <c r="CC24" t="s">
+      <c r="BY24" t="s">
+        <v>1625</v>
+      </c>
+      <c r="BZ24" t="s">
+        <v>82</v>
+      </c>
+      <c r="CE24" t="s">
         <v>191</v>
       </c>
-      <c r="CD24" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="25" spans="3:82">
+      <c r="CF24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="3:84">
       <c r="W25" t="s">
         <v>192</v>
       </c>
@@ -8971,14 +9200,20 @@
       <c r="BH25" t="s">
         <v>82</v>
       </c>
-      <c r="CC25" t="s">
+      <c r="BY25" t="s">
+        <v>1626</v>
+      </c>
+      <c r="BZ25" t="s">
+        <v>82</v>
+      </c>
+      <c r="CE25" t="s">
         <v>192</v>
       </c>
-      <c r="CD25" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="26" spans="3:82">
+      <c r="CF25" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="3:84">
       <c r="W26" t="s">
         <v>193</v>
       </c>
@@ -9051,14 +9286,20 @@
       <c r="BH26" t="s">
         <v>82</v>
       </c>
-      <c r="CC26" t="s">
+      <c r="BY26" t="s">
+        <v>1627</v>
+      </c>
+      <c r="BZ26" t="s">
+        <v>82</v>
+      </c>
+      <c r="CE26" t="s">
         <v>193</v>
       </c>
-      <c r="CD26" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="27" spans="3:82">
+      <c r="CF26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="3:84">
       <c r="W27" t="s">
         <v>194</v>
       </c>
@@ -9131,14 +9372,20 @@
       <c r="BH27" t="s">
         <v>82</v>
       </c>
-      <c r="CC27" t="s">
+      <c r="BY27" t="s">
+        <v>1628</v>
+      </c>
+      <c r="BZ27" t="s">
+        <v>82</v>
+      </c>
+      <c r="CE27" t="s">
         <v>194</v>
       </c>
-      <c r="CD27" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="28" spans="3:82">
+      <c r="CF27" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="3:84">
       <c r="W28" t="s">
         <v>195</v>
       </c>
@@ -9211,14 +9458,14 @@
       <c r="BH28" t="s">
         <v>82</v>
       </c>
-      <c r="CC28" t="s">
+      <c r="CE28" t="s">
         <v>195</v>
       </c>
-      <c r="CD28" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="29" spans="3:82">
+      <c r="CF28" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="3:84">
       <c r="W29" t="s">
         <v>196</v>
       </c>
@@ -9291,14 +9538,14 @@
       <c r="BH29" t="s">
         <v>82</v>
       </c>
-      <c r="CC29" t="s">
+      <c r="CE29" t="s">
         <v>196</v>
       </c>
-      <c r="CD29" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="30" spans="3:82">
+      <c r="CF29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="3:84">
       <c r="W30" t="s">
         <v>197</v>
       </c>
@@ -9371,14 +9618,14 @@
       <c r="BH30" t="s">
         <v>82</v>
       </c>
-      <c r="CC30" t="s">
+      <c r="CE30" t="s">
         <v>197</v>
       </c>
-      <c r="CD30" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="31" spans="3:82">
+      <c r="CF30" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="3:84">
       <c r="W31" t="s">
         <v>198</v>
       </c>
@@ -9451,14 +9698,14 @@
       <c r="BH31" t="s">
         <v>82</v>
       </c>
-      <c r="CC31" t="s">
+      <c r="CE31" t="s">
         <v>198</v>
       </c>
-      <c r="CD31" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="32" spans="3:82">
+      <c r="CF31" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="3:84">
       <c r="W32" t="s">
         <v>199</v>
       </c>
@@ -9531,14 +9778,14 @@
       <c r="BH32" t="s">
         <v>82</v>
       </c>
-      <c r="CC32" t="s">
+      <c r="CE32" t="s">
         <v>199</v>
       </c>
-      <c r="CD32" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="33" spans="23:82">
+      <c r="CF32" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="23:84">
       <c r="W33" t="s">
         <v>200</v>
       </c>
@@ -9611,14 +9858,14 @@
       <c r="BH33" t="s">
         <v>82</v>
       </c>
-      <c r="CC33" t="s">
+      <c r="CE33" t="s">
         <v>200</v>
       </c>
-      <c r="CD33" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="34" spans="23:82">
+      <c r="CF33" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="23:84">
       <c r="W34" t="s">
         <v>201</v>
       </c>
@@ -9691,14 +9938,14 @@
       <c r="BH34" t="s">
         <v>82</v>
       </c>
-      <c r="CC34" t="s">
+      <c r="CE34" t="s">
         <v>201</v>
       </c>
-      <c r="CD34" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="35" spans="23:82">
+      <c r="CF34" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="35" spans="23:84">
       <c r="W35" t="s">
         <v>202</v>
       </c>
@@ -9771,14 +10018,14 @@
       <c r="BH35" t="s">
         <v>82</v>
       </c>
-      <c r="CC35" t="s">
+      <c r="CE35" t="s">
         <v>202</v>
       </c>
-      <c r="CD35" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="36" spans="23:82">
+      <c r="CF35" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="23:84">
       <c r="W36" t="s">
         <v>203</v>
       </c>
@@ -9851,14 +10098,14 @@
       <c r="BH36" t="s">
         <v>82</v>
       </c>
-      <c r="CC36" t="s">
+      <c r="CE36" t="s">
         <v>203</v>
       </c>
-      <c r="CD36" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="37" spans="23:82">
+      <c r="CF36" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="23:84">
       <c r="W37" t="s">
         <v>204</v>
       </c>
@@ -9931,14 +10178,14 @@
       <c r="BH37" t="s">
         <v>82</v>
       </c>
-      <c r="CC37" t="s">
+      <c r="CE37" t="s">
         <v>204</v>
       </c>
-      <c r="CD37" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="38" spans="23:82">
+      <c r="CF37" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="23:84">
       <c r="W38" t="s">
         <v>205</v>
       </c>
@@ -10011,14 +10258,14 @@
       <c r="BH38" t="s">
         <v>82</v>
       </c>
-      <c r="CC38" t="s">
+      <c r="CE38" t="s">
         <v>205</v>
       </c>
-      <c r="CD38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="39" spans="23:82">
+      <c r="CF38" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="39" spans="23:84">
       <c r="W39" t="s">
         <v>206</v>
       </c>
@@ -10091,14 +10338,14 @@
       <c r="BH39" t="s">
         <v>82</v>
       </c>
-      <c r="CC39" t="s">
+      <c r="CE39" t="s">
         <v>206</v>
       </c>
-      <c r="CD39" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="40" spans="23:82">
+      <c r="CF39" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="23:84">
       <c r="W40" t="s">
         <v>207</v>
       </c>
@@ -10171,14 +10418,14 @@
       <c r="BH40" t="s">
         <v>82</v>
       </c>
-      <c r="CC40" t="s">
+      <c r="CE40" t="s">
         <v>207</v>
       </c>
-      <c r="CD40" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="41" spans="23:82">
+      <c r="CF40" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="23:84">
       <c r="W41" t="s">
         <v>208</v>
       </c>
@@ -10251,14 +10498,14 @@
       <c r="BH41" t="s">
         <v>82</v>
       </c>
-      <c r="CC41" t="s">
+      <c r="CE41" t="s">
         <v>208</v>
       </c>
-      <c r="CD41" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="42" spans="23:82">
+      <c r="CF41" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="23:84">
       <c r="W42" t="s">
         <v>209</v>
       </c>
@@ -10331,14 +10578,14 @@
       <c r="BH42" t="s">
         <v>82</v>
       </c>
-      <c r="CC42" t="s">
+      <c r="CE42" t="s">
         <v>209</v>
       </c>
-      <c r="CD42" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="43" spans="23:82">
+      <c r="CF42" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="43" spans="23:84">
       <c r="W43" t="s">
         <v>210</v>
       </c>
@@ -10411,14 +10658,14 @@
       <c r="BH43" t="s">
         <v>82</v>
       </c>
-      <c r="CC43" t="s">
+      <c r="CE43" t="s">
         <v>210</v>
       </c>
-      <c r="CD43" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="44" spans="23:82">
+      <c r="CF43" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" spans="23:84">
       <c r="W44" t="s">
         <v>211</v>
       </c>
@@ -10491,14 +10738,14 @@
       <c r="BH44" t="s">
         <v>82</v>
       </c>
-      <c r="CC44" t="s">
+      <c r="CE44" t="s">
         <v>211</v>
       </c>
-      <c r="CD44" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="45" spans="23:82">
+      <c r="CF44" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="45" spans="23:84">
       <c r="W45" t="s">
         <v>212</v>
       </c>
@@ -10571,14 +10818,14 @@
       <c r="BH45" t="s">
         <v>82</v>
       </c>
-      <c r="CC45" t="s">
+      <c r="CE45" t="s">
         <v>212</v>
       </c>
-      <c r="CD45" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="46" spans="23:82">
+      <c r="CF45" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="46" spans="23:84">
       <c r="W46" t="s">
         <v>213</v>
       </c>
@@ -10651,14 +10898,14 @@
       <c r="BH46" t="s">
         <v>82</v>
       </c>
-      <c r="CC46" t="s">
+      <c r="CE46" t="s">
         <v>213</v>
       </c>
-      <c r="CD46" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="47" spans="23:82">
+      <c r="CF46" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="47" spans="23:84">
       <c r="W47" t="s">
         <v>214</v>
       </c>
@@ -10731,14 +10978,14 @@
       <c r="BH47" t="s">
         <v>82</v>
       </c>
-      <c r="CC47" t="s">
+      <c r="CE47" t="s">
         <v>214</v>
       </c>
-      <c r="CD47" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="48" spans="23:82">
+      <c r="CF47" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="48" spans="23:84">
       <c r="W48" t="s">
         <v>215</v>
       </c>
@@ -10811,14 +11058,14 @@
       <c r="BH48" t="s">
         <v>82</v>
       </c>
-      <c r="CC48" t="s">
+      <c r="CE48" t="s">
         <v>215</v>
       </c>
-      <c r="CD48" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="49" spans="23:82">
+      <c r="CF48" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="49" spans="23:84">
       <c r="W49" t="s">
         <v>216</v>
       </c>
@@ -10891,14 +11138,14 @@
       <c r="BH49" t="s">
         <v>82</v>
       </c>
-      <c r="CC49" t="s">
+      <c r="CE49" t="s">
         <v>216</v>
       </c>
-      <c r="CD49" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="50" spans="23:82">
+      <c r="CF49" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="50" spans="23:84">
       <c r="W50" t="s">
         <v>217</v>
       </c>
@@ -10971,14 +11218,14 @@
       <c r="BH50" t="s">
         <v>82</v>
       </c>
-      <c r="CC50" t="s">
+      <c r="CE50" t="s">
         <v>217</v>
       </c>
-      <c r="CD50" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="51" spans="23:82">
+      <c r="CF50" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="51" spans="23:84">
       <c r="W51" t="s">
         <v>218</v>
       </c>
@@ -11051,14 +11298,14 @@
       <c r="BH51" t="s">
         <v>82</v>
       </c>
-      <c r="CC51" t="s">
+      <c r="CE51" t="s">
         <v>218</v>
       </c>
-      <c r="CD51" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="52" spans="23:82">
+      <c r="CF51" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="52" spans="23:84">
       <c r="W52" t="s">
         <v>219</v>
       </c>
@@ -11131,14 +11378,14 @@
       <c r="BH52" t="s">
         <v>82</v>
       </c>
-      <c r="CC52" t="s">
+      <c r="CE52" t="s">
         <v>219</v>
       </c>
-      <c r="CD52" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="53" spans="23:82">
+      <c r="CF52" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="53" spans="23:84">
       <c r="W53" t="s">
         <v>220</v>
       </c>
@@ -11211,14 +11458,14 @@
       <c r="BH53" t="s">
         <v>82</v>
       </c>
-      <c r="CC53" t="s">
+      <c r="CE53" t="s">
         <v>220</v>
       </c>
-      <c r="CD53" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="54" spans="23:82">
+      <c r="CF53" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="54" spans="23:84">
       <c r="W54" t="s">
         <v>221</v>
       </c>
@@ -11291,14 +11538,14 @@
       <c r="BH54" t="s">
         <v>82</v>
       </c>
-      <c r="CC54" t="s">
+      <c r="CE54" t="s">
         <v>221</v>
       </c>
-      <c r="CD54" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="55" spans="23:82">
+      <c r="CF54" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="55" spans="23:84">
       <c r="W55" t="s">
         <v>222</v>
       </c>
@@ -11371,14 +11618,14 @@
       <c r="BH55" t="s">
         <v>82</v>
       </c>
-      <c r="CC55" t="s">
+      <c r="CE55" t="s">
         <v>222</v>
       </c>
-      <c r="CD55" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="56" spans="23:82">
+      <c r="CF55" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="56" spans="23:84">
       <c r="W56" t="s">
         <v>223</v>
       </c>
@@ -11451,14 +11698,14 @@
       <c r="BH56" t="s">
         <v>82</v>
       </c>
-      <c r="CC56" t="s">
+      <c r="CE56" t="s">
         <v>223</v>
       </c>
-      <c r="CD56" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="57" spans="23:82">
+      <c r="CF56" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="57" spans="23:84">
       <c r="W57" t="s">
         <v>224</v>
       </c>
@@ -11531,14 +11778,14 @@
       <c r="BH57" t="s">
         <v>82</v>
       </c>
-      <c r="CC57" t="s">
+      <c r="CE57" t="s">
         <v>224</v>
       </c>
-      <c r="CD57" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="58" spans="23:82">
+      <c r="CF57" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="58" spans="23:84">
       <c r="W58" t="s">
         <v>225</v>
       </c>
@@ -11611,14 +11858,14 @@
       <c r="BH58" t="s">
         <v>82</v>
       </c>
-      <c r="CC58" t="s">
+      <c r="CE58" t="s">
         <v>225</v>
       </c>
-      <c r="CD58" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="59" spans="23:82">
+      <c r="CF58" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="59" spans="23:84">
       <c r="W59" t="s">
         <v>226</v>
       </c>
@@ -11691,14 +11938,14 @@
       <c r="BH59" t="s">
         <v>82</v>
       </c>
-      <c r="CC59" t="s">
+      <c r="CE59" t="s">
         <v>226</v>
       </c>
-      <c r="CD59" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="60" spans="23:82">
+      <c r="CF59" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="60" spans="23:84">
       <c r="W60" t="s">
         <v>227</v>
       </c>
@@ -11771,14 +12018,14 @@
       <c r="BH60" t="s">
         <v>82</v>
       </c>
-      <c r="CC60" t="s">
+      <c r="CE60" t="s">
         <v>227</v>
       </c>
-      <c r="CD60" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="61" spans="23:82">
+      <c r="CF60" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="61" spans="23:84">
       <c r="AK61" t="s">
         <v>424</v>
       </c>
@@ -11834,7 +12081,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="62" spans="23:82">
+    <row r="62" spans="23:84">
       <c r="AK62" t="s">
         <v>425</v>
       </c>
@@ -11890,7 +12137,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="63" spans="23:82">
+    <row r="63" spans="23:84">
       <c r="AK63" t="s">
         <v>426</v>
       </c>
@@ -11946,7 +12193,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="64" spans="23:82">
+    <row r="64" spans="23:84">
       <c r="AK64" t="s">
         <v>427</v>
       </c>
@@ -34885,7 +35132,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="47">
+  <mergeCells count="48">
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
@@ -34932,10 +35179,11 @@
     <mergeCell ref="BY2:BZ2"/>
     <mergeCell ref="CA2:CB2"/>
     <mergeCell ref="CC2:CD2"/>
-    <mergeCell ref="BY1:CD1"/>
+    <mergeCell ref="CE2:CF2"/>
+    <mergeCell ref="BY1:CF1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="41">
+  <tableParts count="42">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
@@ -34977,6 +35225,7 @@
     <tablePart r:id="rId39"/>
     <tablePart r:id="rId40"/>
     <tablePart r:id="rId41"/>
+    <tablePart r:id="rId42"/>
   </tableParts>
 </worksheet>
 </file>
@@ -38005,7 +38254,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -38014,23 +38263,25 @@
     <col min="1" max="1" width="8.7109375" style="2" customWidth="1"/>
     <col min="2" max="3" width="26.7109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="30.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="52.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="22.7109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" style="2" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="34.7109375" style="2" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="26.7109375" style="2" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="44.7109375" style="3" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="42.7109375" style="5" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="48.7109375" style="2" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="40.7109375" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="40.7109375" style="2" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="44.7109375" style="2" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="36.7109375" style="2" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="2" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="24.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="56.7109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="26.7109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" style="2" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="26.7109375" style="2" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="26.7109375" style="3" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="24.7109375" style="5" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="30.7109375" style="2" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="22.7109375" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="24.7109375" style="2" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="44.7109375" style="2" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="36.7109375" style="2" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" hidden="1">
+    <row r="1" spans="1:20" hidden="1">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -38047,46 +38298,52 @@
         <v>1594</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1595</v>
+        <v>1596</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1596</v>
+        <v>1599</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>1597</v>
+        <v>1600</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>1601</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>1602</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>1603</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>1599</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:18" hidden="1">
+    <row r="2" spans="1:20" hidden="1">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -38100,35 +38357,39 @@
         <v>53</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>1594</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>1595</v>
-      </c>
+        <v>1598</v>
+      </c>
+      <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>1598</v>
-      </c>
-      <c r="H2" s="1"/>
+        <v>1599</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>1600</v>
+      </c>
       <c r="I2" s="1" t="s">
+        <v>1601</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>1604</v>
+      </c>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>1601</v>
-      </c>
-      <c r="K2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
-      <c r="Q2" s="1" t="s">
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="R2" s="1"/>
-    </row>
-    <row r="3" spans="1:18" hidden="1">
+      <c r="T2" s="1"/>
+    </row>
+    <row r="3" spans="1:20" hidden="1">
       <c r="B3" s="7" t="s">
         <v>11</v>
       </c>
@@ -38138,37 +38399,40 @@
       <c r="D3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="E3" s="1" t="s">
+        <v>1595</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>1597</v>
+      </c>
+      <c r="J3" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="K3" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>1600</v>
-      </c>
-      <c r="K3" s="7" t="s">
+      <c r="M3" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="N3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7" t="s">
+      <c r="O3" s="7"/>
+      <c r="P3" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="O3" s="7"/>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="7"/>
+      <c r="R3" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="Q3" s="7" t="s">
+      <c r="S3" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:18" hidden="1">
+    <row r="4" spans="1:20" hidden="1">
       <c r="B4" s="7" t="s">
         <v>0</v>
       </c>
@@ -38178,20 +38442,20 @@
       <c r="D4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="P4" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="O4" s="7" t="s">
+      <c r="Q4" s="7" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:20">
       <c r="A5" s="6" t="s">
         <v>0</v>
       </c>
@@ -38205,80 +38469,91 @@
         <v>53</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>1595</v>
+        <v>1597</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>1596</v>
+        <v>1599</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>1597</v>
+        <v>1600</v>
       </c>
       <c r="I5" s="1" t="s">
+        <v>1601</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>1599</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="M5" s="1" t="s">
-        <v>68</v>
+        <v>165</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>62</v>
+        <v>168</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>64</v>
+        <v>169</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>70</v>
+        <v>166</v>
       </c>
       <c r="Q5" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="S5" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="R5" s="1" t="s">
+      <c r="T5" s="1" t="s">
         <v>78</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="L3:M3"/>
+  <mergeCells count="6">
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="J2:K2"/>
     <mergeCell ref="N3:O3"/>
-    <mergeCell ref="K2:P2"/>
-    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="M2:R2"/>
+    <mergeCell ref="S2:T2"/>
   </mergeCells>
-  <dataValidations count="6">
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:E1000001">
+  <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:E1000001">
+      <formula1>'Codelijsten'!$BY$4:$BY$27</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F1000001">
+      <formula1>'Codelijsten'!$CA$4:$CA$17</formula1>
+    </dataValidation>
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G1000001">
       <formula1>-146096</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F1000001">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H6:H1000001">
       <formula1>-146096</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I6:I1000001">
-      <formula1>'Codelijsten'!$BY$4:$BY$8</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L6:L1000001">
+      <formula1>'Codelijsten'!$CC$4:$CC$8</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J6:J1000001">
-      <formula1>'Codelijsten'!$CA$4:$CA$17</formula1>
-    </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L6:L1000001">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N6:N1000001">
       <formula1>-146096</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P6:P1000001">
-      <formula1>'Codelijsten'!$CC$4:$CC$60</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R6:R1000001">
+      <formula1>'Codelijsten'!$CE$4:$CE$60</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="I5" location="'Codelijsten'!$BY$2" display="status"/>
-    <hyperlink ref="J5" location="'Codelijsten'!$CA$2" display="kwaliteit-origine"/>
-    <hyperlink ref="P5" location="'Codelijsten'!$CC$2" display="bijlage-bijlage_type"/>
+    <hyperlink ref="E5" location="'Codelijsten'!$BY$2" display="aard"/>
+    <hyperlink ref="F5" location="'Codelijsten'!$CA$2" display="origine"/>
+    <hyperlink ref="L5" location="'Codelijsten'!$CC$2" display="status"/>
+    <hyperlink ref="R5" location="'Codelijsten'!$CE$2" display="type bijlage"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -38294,26 +38569,26 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>1615</v>
+        <v>1642</v>
       </c>
       <c r="B1" t="s">
-        <v>1616</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>1617</v>
+        <v>1644</v>
       </c>
       <c r="B2" t="s">
-        <v>1618</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>1619</v>
+        <v>1646</v>
       </c>
       <c r="B3" t="s">
-        <v>1620</v>
+        <v>1647</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made header height more consistent in xls-templates
</commit_message>
<xml_diff>
--- a/data/bodem_template.xlsx
+++ b/data/bodem_template.xlsx
@@ -4952,7 +4952,7 @@
     <t>Date generated</t>
   </si>
   <si>
-    <t>2024-07-24 13:26:29.895029</t>
+    <t>2024-08-01 09:38:05.454480</t>
   </si>
   <si>
     <t>version</t>
@@ -35232,7 +35232,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AU8"/>
+  <dimension ref="A1:AU9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -35732,146 +35732,147 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:47">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:47" hidden="1"/>
+    <row r="9" spans="1:47">
+      <c r="A9" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B9" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C9" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D9" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E9" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F9" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G9" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H9" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I9" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J9" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="K9" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="L8" s="6" t="s">
+      <c r="L9" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="M8" s="6" t="s">
+      <c r="M9" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="N9" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="O9" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="P9" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="Q9" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="R8" s="1" t="s">
+      <c r="R9" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="S8" s="1" t="s">
+      <c r="S9" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="T8" s="1" t="s">
+      <c r="T9" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="U8" s="1" t="s">
+      <c r="U9" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="V8" s="1" t="s">
+      <c r="V9" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="W8" s="1" t="s">
+      <c r="W9" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="X8" s="1" t="s">
+      <c r="X9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Y8" s="1" t="s">
+      <c r="Y9" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="Z8" s="1" t="s">
+      <c r="Z9" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="AA8" s="1" t="s">
+      <c r="AA9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AB8" s="1" t="s">
+      <c r="AB9" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="AC8" s="1" t="s">
+      <c r="AC9" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="AD8" s="1" t="s">
+      <c r="AD9" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AE8" s="1" t="s">
+      <c r="AE9" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AF8" s="1" t="s">
+      <c r="AF9" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AG8" s="1" t="s">
+      <c r="AG9" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="AH8" s="1" t="s">
+      <c r="AH9" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AI8" s="1" t="s">
+      <c r="AI9" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="AJ8" s="1" t="s">
+      <c r="AJ9" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="AK8" s="1" t="s">
+      <c r="AK9" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="AL8" s="1" t="s">
+      <c r="AL9" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="AM8" s="1" t="s">
+      <c r="AM9" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="AN8" s="1" t="s">
+      <c r="AN9" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="AO8" s="1" t="s">
+      <c r="AO9" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="AP8" s="1" t="s">
+      <c r="AP9" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="AQ8" s="1" t="s">
+      <c r="AQ9" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="AR8" s="1" t="s">
+      <c r="AR9" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="AS8" s="1" t="s">
+      <c r="AS9" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="AT8" s="1" t="s">
+      <c r="AT9" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="AU8" s="1" t="s">
+      <c r="AU9" s="1" t="s">
         <v>78</v>
       </c>
     </row>
@@ -35894,71 +35895,71 @@
     <mergeCell ref="AT2:AU2"/>
   </mergeCells>
   <dataValidations count="17">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:B1000001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10:B1000001">
       <formula1>'Codelijsten'!$A$4:$A$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C1000001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10:C1000001">
       <formula1>'Codelijsten'!$C$4:$C$21</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:D1000001">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10:D1000001">
       <formula1>-146096</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G9:G1000001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G10:G1000001">
       <formula1>'Codelijsten'!$E$4:$E$17</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I9:I1000001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I10:I1000001">
       <formula1>'Codelijsten'!$G$4:$G$6</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K9:K1000001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K10:K1000001">
       <formula1>'Codelijsten'!$I$4:$I$20</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M9:M1000001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M10:M1000001">
       <formula1>'Codelijsten'!$K$4:$K$6</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P9:P1000001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P10:P1000001">
       <formula1>'Codelijsten'!$M$4:$M$6</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q9:Q1000001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q10:Q1000001">
       <formula1>'Codelijsten'!$O$4:$O$17</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T9:T1000001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T10:T1000001">
       <formula1>'Codelijsten'!$Q$4:$Q$6</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U9:U1000001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U10:U1000001">
       <formula1>'Codelijsten'!$S$4:$S$20</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W9:W1000001">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W10:W1000001">
       <formula1>-146096</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE9:AE1000001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE10:AE1000001">
       <formula1>'Codelijsten'!$U$4:$U$8</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF9:AF1000001">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF10:AF1000001">
       <formula1>-146096</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK9:AK1000001">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK10:AK1000001">
       <formula1>-146096</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO9:AO1000001">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO10:AO1000001">
       <formula1>-146096</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ9:AQ1000001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ10:AQ1000001">
       <formula1>'Codelijsten'!$W$4:$W$60</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B8" location="'Codelijsten'!$A$2" display="type"/>
-    <hyperlink ref="C8" location="'Codelijsten'!$C$2" display="doel"/>
-    <hyperlink ref="G8" location="'Codelijsten'!$E$2" display="methode opmeten xy-coördinaten beginpunt"/>
-    <hyperlink ref="I8" location="'Codelijsten'!$G$2" display="betrouwbaarheid xy-coördinaten beginpunt"/>
-    <hyperlink ref="K8" location="'Codelijsten'!$I$2" display="methode opmeten maaiveld beginpunt"/>
-    <hyperlink ref="M8" location="'Codelijsten'!$K$2" display="betrouwbaarheid maaiveld beginpunt"/>
-    <hyperlink ref="P8" location="'Codelijsten'!$M$2" display="betrouwbaarheid xy-coördinaten eindpunt"/>
-    <hyperlink ref="Q8" location="'Codelijsten'!$O$2" display="methode opmeten xy-coördinaten eindpunt"/>
-    <hyperlink ref="T8" location="'Codelijsten'!$Q$2" display="betrouwbaarheid maaiveld eindpunt"/>
-    <hyperlink ref="U8" location="'Codelijsten'!$S$2" display="methode opmeten maaiveld eindpunt"/>
-    <hyperlink ref="AE8" location="'Codelijsten'!$U$2" display="status"/>
-    <hyperlink ref="AQ8" location="'Codelijsten'!$W$2" display="type bijlage"/>
+    <hyperlink ref="B9" location="'Codelijsten'!$A$2" display="type"/>
+    <hyperlink ref="C9" location="'Codelijsten'!$C$2" display="doel"/>
+    <hyperlink ref="G9" location="'Codelijsten'!$E$2" display="methode opmeten xy-coördinaten beginpunt"/>
+    <hyperlink ref="I9" location="'Codelijsten'!$G$2" display="betrouwbaarheid xy-coördinaten beginpunt"/>
+    <hyperlink ref="K9" location="'Codelijsten'!$I$2" display="methode opmeten maaiveld beginpunt"/>
+    <hyperlink ref="M9" location="'Codelijsten'!$K$2" display="betrouwbaarheid maaiveld beginpunt"/>
+    <hyperlink ref="P9" location="'Codelijsten'!$M$2" display="betrouwbaarheid xy-coördinaten eindpunt"/>
+    <hyperlink ref="Q9" location="'Codelijsten'!$O$2" display="methode opmeten xy-coördinaten eindpunt"/>
+    <hyperlink ref="T9" location="'Codelijsten'!$Q$2" display="betrouwbaarheid maaiveld eindpunt"/>
+    <hyperlink ref="U9" location="'Codelijsten'!$S$2" display="methode opmeten maaiveld eindpunt"/>
+    <hyperlink ref="AE9" location="'Codelijsten'!$U$2" display="status"/>
+    <hyperlink ref="AQ9" location="'Codelijsten'!$W$2" display="type bijlage"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -35966,7 +35967,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y6"/>
+  <dimension ref="A1:Y7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -36210,80 +36211,81 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:25" hidden="1"/>
+    <row r="7" spans="1:25">
+      <c r="A7" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="O7" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="P7" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="Q7" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="R6" s="1" t="s">
+      <c r="R7" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="S6" s="1" t="s">
+      <c r="S7" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="T6" s="1" t="s">
+      <c r="T7" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="U6" s="1" t="s">
+      <c r="U7" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="V6" s="1" t="s">
+      <c r="V7" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="W6" s="1" t="s">
+      <c r="W7" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="X6" s="1" t="s">
+      <c r="X7" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="Y6" s="1" t="s">
+      <c r="Y7" s="1" t="s">
         <v>78</v>
       </c>
     </row>
@@ -36300,28 +36302,28 @@
     <mergeCell ref="X2:Y2"/>
   </mergeCells>
   <dataValidations count="6">
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:C1000001">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:C1000001">
       <formula1>-146096</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I7:I1000001">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I8:I1000001">
       <formula1>-146096</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K7:K1000001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K8:K1000001">
       <formula1>'Codelijsten'!$Y$4:$Y$8</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O7:O1000001">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O8:O1000001">
       <formula1>-146096</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S7:S1000001">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S8:S1000001">
       <formula1>-146096</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U7:U1000001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U8:U1000001">
       <formula1>'Codelijsten'!$AA$4:$AA$60</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="K6" location="'Codelijsten'!$Y$2" display="status"/>
-    <hyperlink ref="U6" location="'Codelijsten'!$AA$2" display="type bijlage"/>
+    <hyperlink ref="K7" location="'Codelijsten'!$Y$2" display="status"/>
+    <hyperlink ref="U7" location="'Codelijsten'!$AA$2" display="type bijlage"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -37827,7 +37829,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB7"/>
+  <dimension ref="A1:AB8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -38116,89 +38118,90 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:28">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:28" hidden="1"/>
+    <row r="8" spans="1:28">
+      <c r="A8" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B8" s="6" t="s">
         <v>1553</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C8" s="6" t="s">
         <v>1554</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>1555</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>1556</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>1557</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>1558</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>1559</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>1560</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>1529</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="N8" s="1" t="s">
         <v>1563</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="O8" s="1" t="s">
         <v>1564</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="P8" s="1" t="s">
         <v>1565</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="Q8" s="1" t="s">
         <v>1566</v>
       </c>
-      <c r="R7" s="1" t="s">
+      <c r="R8" s="1" t="s">
         <v>1567</v>
       </c>
-      <c r="S7" s="1" t="s">
+      <c r="S8" s="1" t="s">
         <v>1568</v>
       </c>
-      <c r="T7" s="1" t="s">
+      <c r="T8" s="1" t="s">
         <v>1569</v>
       </c>
-      <c r="U7" s="1" t="s">
+      <c r="U8" s="1" t="s">
         <v>1570</v>
       </c>
-      <c r="V7" s="1" t="s">
+      <c r="V8" s="1" t="s">
         <v>1577</v>
       </c>
-      <c r="W7" s="1" t="s">
+      <c r="W8" s="1" t="s">
         <v>1582</v>
       </c>
-      <c r="X7" s="1" t="s">
+      <c r="X8" s="1" t="s">
         <v>1583</v>
       </c>
-      <c r="Y7" s="1" t="s">
+      <c r="Y8" s="1" t="s">
         <v>1584</v>
       </c>
-      <c r="Z7" s="1" t="s">
+      <c r="Z8" s="1" t="s">
         <v>1585</v>
       </c>
-      <c r="AA7" s="1" t="s">
+      <c r="AA8" s="1" t="s">
         <v>1586</v>
       </c>
-      <c r="AB7" s="1" t="s">
+      <c r="AB8" s="1" t="s">
         <v>1587</v>
       </c>
     </row>
@@ -38215,38 +38218,38 @@
     <mergeCell ref="K2:AB2"/>
   </mergeCells>
   <dataValidations count="8">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B1000001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:B1000001">
       <formula1>'Codelijsten'!$BM$4:$BM$6</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:C1000001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C1000001">
       <formula1>'Codelijsten'!$BO$4:$BO$6</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H8:H1000001">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H9:H1000001">
       <formula1>-146096</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K8:K1000001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K9:K1000001">
       <formula1>'Codelijsten'!$BQ$4:$BQ$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M8:M1000001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M9:M1000001">
       <formula1>'Codelijsten'!$BS$4:$BS$6</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U8:U1000001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U9:U1000001">
       <formula1>'Codelijsten'!$BU$4:$BU$9</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V8:V1000001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V9:V1000001">
       <formula1>'Codelijsten'!$BW$4:$BW$7</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X8:X1000001">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X9:X1000001">
       <formula1>-146096</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B7" location="'Codelijsten'!$BM$2" display="type metadata"/>
-    <hyperlink ref="C7" location="'Codelijsten'!$BO$2" display="betrouwbaarheid metadata"/>
-    <hyperlink ref="K7" location="'Codelijsten'!$BQ$2" display="type diepteinterval"/>
-    <hyperlink ref="M7" location="'Codelijsten'!$BS$2" display="diepteinterval-beschrijving-type"/>
-    <hyperlink ref="U7" location="'Codelijsten'!$BU$2" display="grensduidelijkheid diepteinterval"/>
-    <hyperlink ref="V7" location="'Codelijsten'!$BW$2" display="grensregelmatigheid diepteinterval"/>
+    <hyperlink ref="B8" location="'Codelijsten'!$BM$2" display="type metadata"/>
+    <hyperlink ref="C8" location="'Codelijsten'!$BO$2" display="betrouwbaarheid metadata"/>
+    <hyperlink ref="K8" location="'Codelijsten'!$BQ$2" display="type diepteinterval"/>
+    <hyperlink ref="M8" location="'Codelijsten'!$BS$2" display="diepteinterval-beschrijving-type"/>
+    <hyperlink ref="U8" location="'Codelijsten'!$BU$2" display="grensduidelijkheid diepteinterval"/>
+    <hyperlink ref="V8" location="'Codelijsten'!$BW$2" display="grensregelmatigheid diepteinterval"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -38254,7 +38257,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T5"/>
+  <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -38455,65 +38458,66 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:20" hidden="1"/>
+    <row r="6" spans="1:20">
+      <c r="A6" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B6" s="6" t="s">
         <v>1590</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C6" s="6" t="s">
         <v>1592</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>1595</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>1597</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>1599</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>1600</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>1601</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="O6" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="P6" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="Q6" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="R5" s="1" t="s">
+      <c r="R6" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="S5" s="1" t="s">
+      <c r="S6" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="T5" s="1" t="s">
+      <c r="T6" s="1" t="s">
         <v>78</v>
       </c>
     </row>
@@ -38527,33 +38531,33 @@
     <mergeCell ref="S2:T2"/>
   </mergeCells>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:E1000001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E1000001">
       <formula1>'Codelijsten'!$BY$4:$BY$27</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F1000001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F7:F1000001">
       <formula1>'Codelijsten'!$CA$4:$CA$17</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G1000001">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G7:G1000001">
       <formula1>-146096</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H6:H1000001">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H1000001">
       <formula1>-146096</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L6:L1000001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L7:L1000001">
       <formula1>'Codelijsten'!$CC$4:$CC$8</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N6:N1000001">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N7:N1000001">
       <formula1>-146096</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R6:R1000001">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R7:R1000001">
       <formula1>'Codelijsten'!$CE$4:$CE$60</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E5" location="'Codelijsten'!$BY$2" display="aard"/>
-    <hyperlink ref="F5" location="'Codelijsten'!$CA$2" display="origine"/>
-    <hyperlink ref="L5" location="'Codelijsten'!$CC$2" display="status"/>
-    <hyperlink ref="R5" location="'Codelijsten'!$CE$2" display="type bijlage"/>
+    <hyperlink ref="E6" location="'Codelijsten'!$BY$2" display="aard"/>
+    <hyperlink ref="F6" location="'Codelijsten'!$CA$2" display="origine"/>
+    <hyperlink ref="L6" location="'Codelijsten'!$CC$2" display="status"/>
+    <hyperlink ref="R6" location="'Codelijsten'!$CE$2" display="type bijlage"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added option to convert templates in other environments (ontwikkel, oefen)
</commit_message>
<xml_diff>
--- a/data/bodem_template.xlsx
+++ b/data/bodem_template.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9957" uniqueCount="1645">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9961" uniqueCount="1649">
   <si>
     <t>naam</t>
   </si>
@@ -4949,13 +4949,25 @@
     <t>Date generated</t>
   </si>
   <si>
-    <t>2024-08-05 10:13:25.299893</t>
+    <t>2024-08-07 13:31:38.616168</t>
   </si>
   <si>
     <t>version</t>
   </si>
   <si>
     <t>2.0.0</t>
+  </si>
+  <si>
+    <t>mode</t>
+  </si>
+  <si>
+    <t>local</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>xsd_schema.json</t>
   </si>
 </sst>
 </file>
@@ -38556,7 +38568,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -38578,6 +38590,22 @@
         <v>1644</v>
       </c>
     </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>1645</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1646</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>1647</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1648</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Small bugfix to use oefen-xsd
</commit_message>
<xml_diff>
--- a/data/bodem_template.xlsx
+++ b/data/bodem_template.xlsx
@@ -4949,13 +4949,13 @@
     <t>Date generated</t>
   </si>
   <si>
-    <t>2024-08-08 11:46:47.802569</t>
+    <t>2024-08-12 14:45:30.853850</t>
   </si>
   <si>
     <t>version</t>
   </si>
   <si>
-    <t>2.0.0</t>
+    <t>2.0.1</t>
   </si>
   <si>
     <t>mode</t>
@@ -4967,7 +4967,7 @@
     <t>source</t>
   </si>
   <si>
-    <t>xsd_schema.json</t>
+    <t>productie</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Quick fix to ontwikkel schema
</commit_message>
<xml_diff>
--- a/data/bodem_template.xlsx
+++ b/data/bodem_template.xlsx
@@ -5258,7 +5258,7 @@
     <t>Date generated</t>
   </si>
   <si>
-    <t>2024-11-08 02:13:54.487394</t>
+    <t>2024-11-08 08:59:54.364436</t>
   </si>
   <si>
     <t>version</t>
@@ -5270,7 +5270,7 @@
     <t>mode</t>
   </si>
   <si>
-    <t>local</t>
+    <t>online</t>
   </si>
   <si>
     <t>source</t>

</xml_diff>

<commit_message>
Added diepte to grondwaterlocatie sheet in grondwater_template.xlsx
</commit_message>
<xml_diff>
--- a/data/bodem_template.xlsx
+++ b/data/bodem_template.xlsx
@@ -5282,13 +5282,13 @@
     <t>Date generated</t>
   </si>
   <si>
-    <t>2024-11-12 08:42:19.421207</t>
+    <t>2024-12-02 16:44:12.447900</t>
   </si>
   <si>
     <t>version</t>
   </si>
   <si>
-    <t>2.0.4</t>
+    <t>2.0.5</t>
   </si>
   <si>
     <t>mode</t>

</xml_diff>

<commit_message>
Made date reading less prone to errors
</commit_message>
<xml_diff>
--- a/data/bodem_template.xlsx
+++ b/data/bodem_template.xlsx
@@ -5282,13 +5282,13 @@
     <t>Date generated</t>
   </si>
   <si>
-    <t>2024-12-02 16:44:12.447900</t>
+    <t>2024-12-10 17:55:18.947026</t>
   </si>
   <si>
     <t>version</t>
   </si>
   <si>
-    <t>2.0.5</t>
+    <t>2.0.6</t>
   </si>
   <si>
     <t>mode</t>

</xml_diff>

<commit_message>
Fixed small error catching bug
</commit_message>
<xml_diff>
--- a/data/bodem_template.xlsx
+++ b/data/bodem_template.xlsx
@@ -5282,13 +5282,13 @@
     <t>Date generated</t>
   </si>
   <si>
-    <t>2024-12-10 17:55:18.947026</t>
+    <t>2024-12-20 12:16:40.875871</t>
   </si>
   <si>
     <t>version</t>
   </si>
   <si>
-    <t>2.0.6</t>
+    <t>2.0.7</t>
   </si>
   <si>
     <t>mode</t>

</xml_diff>

<commit_message>
Small update to ontwikkel xsd
</commit_message>
<xml_diff>
--- a/data/bodem_template.xlsx
+++ b/data/bodem_template.xlsx
@@ -5282,13 +5282,13 @@
     <t>Date generated</t>
   </si>
   <si>
-    <t>2024-12-20 14:58:10.084591</t>
+    <t>2024-12-23 11:42:04.362622</t>
   </si>
   <si>
     <t>version</t>
   </si>
   <si>
-    <t>2.0.7</t>
+    <t>2.0.8</t>
   </si>
   <si>
     <t>mode</t>

</xml_diff>

<commit_message>
added new info to config and metadata-sheet
</commit_message>
<xml_diff>
--- a/data/bodem_template.xlsx
+++ b/data/bodem_template.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6784" uniqueCount="1762">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6786" uniqueCount="1764">
   <si>
     <t>naam</t>
   </si>
@@ -5282,7 +5282,7 @@
     <t>Date generated</t>
   </si>
   <si>
-    <t>2025-02-14 13:20:02.412411</t>
+    <t>2025-02-14 14:05:32.524017</t>
   </si>
   <si>
     <t>version</t>
@@ -5291,10 +5291,16 @@
     <t>2.0.9</t>
   </si>
   <si>
-    <t>xsd-version</t>
+    <t>xdov-version</t>
   </si>
   <si>
     <t>9.1.0</t>
+  </si>
+  <si>
+    <t>schema-version</t>
+  </si>
+  <si>
+    <t>5.4.0</t>
   </si>
   <si>
     <t>mode</t>
@@ -29456,7 +29462,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -29502,6 +29508,14 @@
         <v>1761</v>
       </c>
     </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>1762</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1763</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Speed up of xls2xml
</commit_message>
<xml_diff>
--- a/data/bodem_template.xlsx
+++ b/data/bodem_template.xlsx
@@ -5282,13 +5282,13 @@
     <t>Date generated</t>
   </si>
   <si>
-    <t>2025-02-14 14:05:32.524017</t>
+    <t>2025-02-24 16:59:54.342594</t>
   </si>
   <si>
     <t>version</t>
   </si>
   <si>
-    <t>2.0.9</t>
+    <t>2.1.0</t>
   </si>
   <si>
     <t>xdov-version</t>

</xml_diff>

<commit_message>
Added observatie and monster sheets to template_full.xlsx
</commit_message>
<xml_diff>
--- a/data/bodem_template.xlsx
+++ b/data/bodem_template.xlsx
@@ -5282,13 +5282,13 @@
     <t>Date generated</t>
   </si>
   <si>
-    <t>2025-02-24 16:59:54.342594</t>
+    <t>2025-02-28 11:24:48.099388</t>
   </si>
   <si>
     <t>version</t>
   </si>
   <si>
-    <t>2.1.0</t>
+    <t>2.1.1</t>
   </si>
   <si>
     <t>xdov-version</t>

</xml_diff>